<commit_message>
he hecho algunos avances
</commit_message>
<xml_diff>
--- a/Excel/matriz_tabla_contingencia.xlsx
+++ b/Excel/matriz_tabla_contingencia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\MASTER\TFM\rTFM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\MASTER\TFM\rTFM\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="USOS_GENERAL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="58">
   <si>
     <t>Agrario</t>
   </si>
@@ -136,6 +136,69 @@
   </si>
   <si>
     <t>Zonas en construcción</t>
+  </si>
+  <si>
+    <t>Sin asignacion</t>
+  </si>
+  <si>
+    <t>Tejido urbano</t>
+  </si>
+  <si>
+    <t>Zonas industriales y comerciales</t>
+  </si>
+  <si>
+    <t>Infraestructuras de comunicaciones</t>
+  </si>
+  <si>
+    <t>Otras infraestructuras tecnicas</t>
+  </si>
+  <si>
+    <t>Zonas mineras, escombreras o de vertido</t>
+  </si>
+  <si>
+    <t>Zonas verdes y espacios de ocio</t>
+  </si>
+  <si>
+    <t>Mares y oceanos</t>
+  </si>
+  <si>
+    <t>Rios, cauces o ramblas</t>
+  </si>
+  <si>
+    <t>Vegetacion riparia</t>
+  </si>
+  <si>
+    <t>Lagos y lagunas</t>
+  </si>
+  <si>
+    <t>Masas de agua artificial</t>
+  </si>
+  <si>
+    <t>Leñoso secano</t>
+  </si>
+  <si>
+    <t>Leñoso regadio</t>
+  </si>
+  <si>
+    <t>Cultivos herbaceos</t>
+  </si>
+  <si>
+    <t>Areas agrarias heterogeneas</t>
+  </si>
+  <si>
+    <t>Vegetacion natural</t>
+  </si>
+  <si>
+    <t>Vegetación con eucaliptos</t>
+  </si>
+  <si>
+    <t>Playas, dunas y arenales</t>
+  </si>
+  <si>
+    <t>Areas con fuertes procesos erosivos</t>
+  </si>
+  <si>
+    <t>Zonas en construccion</t>
   </si>
 </sst>
 </file>
@@ -549,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -642,6 +705,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -931,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1234,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE419"/>
+  <dimension ref="A1:DF419"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH1:AO2"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="CT1" sqref="CT1:CT1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,9 +1321,11 @@
     <col min="23" max="24" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4" bestFit="1" customWidth="1"/>
     <col min="26" max="29" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="84" width="3.5703125" customWidth="1"/>
+    <col min="86" max="109" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="199.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:110" ht="199.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="28"/>
       <c r="H1" s="39" t="s">
         <v>26</v>
@@ -1391,8 +1459,150 @@
       <c r="BD1" s="41" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BI1" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="BJ1" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="BK1" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL1" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="BM1" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN1" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="BO1" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="BP1" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="BQ1" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="BR1" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="BS1" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="BT1" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="BU1" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="BV1" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="BW1" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="BX1" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="BY1" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="BZ1" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="CA1" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="CB1" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="CC1" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="CD1" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="CE1" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="CF1" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="CH1" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="CI1" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="CJ1" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="CK1" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="CL1" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="CM1" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="CN1" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="CO1" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="CP1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="CQ1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="CR1" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="CS1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="CT1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="CU1" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="CV1" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="CW1" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="CX1" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="CY1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="CZ1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="DA1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="DB1" s="40"/>
+      <c r="DC1" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="DD1" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="DE1" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1554,8 +1764,88 @@
         <f>SUM(AI2:BD2)</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH2" t="s">
+        <v>37</v>
+      </c>
+      <c r="CG2" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="CH2" s="32">
+        <v>2</v>
+      </c>
+      <c r="CI2" s="31">
+        <v>2</v>
+      </c>
+      <c r="CJ2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CK2" s="32">
+        <v>3</v>
+      </c>
+      <c r="CL2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CM2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CN2" s="33">
+        <v>0</v>
+      </c>
+      <c r="CO2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CP2" s="32">
+        <v>6</v>
+      </c>
+      <c r="CQ2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CR2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CS2" s="32">
+        <v>5</v>
+      </c>
+      <c r="CT2" s="32">
+        <v>31</v>
+      </c>
+      <c r="CU2" s="32">
+        <v>11</v>
+      </c>
+      <c r="CV2" s="32">
+        <v>4</v>
+      </c>
+      <c r="CW2" s="32">
+        <v>0</v>
+      </c>
+      <c r="CX2" s="32">
+        <v>7</v>
+      </c>
+      <c r="CY2" s="32">
+        <v>36</v>
+      </c>
+      <c r="CZ2" s="32">
+        <v>23</v>
+      </c>
+      <c r="DA2" s="32">
+        <v>1</v>
+      </c>
+      <c r="DB2" s="32"/>
+      <c r="DC2" s="32">
+        <v>0</v>
+      </c>
+      <c r="DD2" s="32">
+        <v>36</v>
+      </c>
+      <c r="DE2" s="32">
+        <v>13</v>
+      </c>
+      <c r="DF2" s="5">
+        <f>SUM(CI2:DE2)</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1717,8 +2007,88 @@
         <f t="shared" ref="BE3:BE21" si="1">SUM(AI3:BD3)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH3" t="s">
+        <v>38</v>
+      </c>
+      <c r="CG3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="CH3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI3" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="30">
+        <v>1</v>
+      </c>
+      <c r="CN3" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS3" s="30">
+        <v>2</v>
+      </c>
+      <c r="CT3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY3" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA3" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB3" s="30"/>
+      <c r="DC3" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD3" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE3" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="7">
+        <f>SUM(CI3:DE3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1880,8 +2250,88 @@
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH4" t="s">
+        <v>39</v>
+      </c>
+      <c r="CG4" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="CH4" s="30">
+        <v>16</v>
+      </c>
+      <c r="CI4" s="34">
+        <v>2</v>
+      </c>
+      <c r="CJ4" s="30">
+        <v>1</v>
+      </c>
+      <c r="CK4" s="30">
+        <v>9</v>
+      </c>
+      <c r="CL4" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM4" s="30">
+        <v>1</v>
+      </c>
+      <c r="CN4" s="35">
+        <v>4</v>
+      </c>
+      <c r="CO4" s="30">
+        <v>2</v>
+      </c>
+      <c r="CP4" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS4" s="30">
+        <v>18</v>
+      </c>
+      <c r="CT4" s="30">
+        <v>26</v>
+      </c>
+      <c r="CU4" s="30">
+        <v>31</v>
+      </c>
+      <c r="CV4" s="30">
+        <v>15</v>
+      </c>
+      <c r="CW4" s="30">
+        <v>28</v>
+      </c>
+      <c r="CX4" s="30">
+        <v>3</v>
+      </c>
+      <c r="CY4" s="30">
+        <v>11</v>
+      </c>
+      <c r="CZ4" s="30">
+        <v>9</v>
+      </c>
+      <c r="DA4" s="30">
+        <v>8</v>
+      </c>
+      <c r="DB4" s="30"/>
+      <c r="DC4" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD4" s="30">
+        <v>46</v>
+      </c>
+      <c r="DE4" s="30">
+        <v>10</v>
+      </c>
+      <c r="DF4" s="7">
+        <f>SUM(CI4:DE4)</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2043,8 +2493,88 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH5" t="s">
+        <v>40</v>
+      </c>
+      <c r="CG5" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="CH5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI5" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="35">
+        <v>1</v>
+      </c>
+      <c r="CO5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS5" s="30">
+        <v>1</v>
+      </c>
+      <c r="CT5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY5" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB5" s="30"/>
+      <c r="DC5" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD5" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE5" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF5" s="7">
+        <f>SUM(CI5:DE5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2206,8 +2736,88 @@
         <f t="shared" si="1"/>
         <v>290</v>
       </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH6" t="s">
+        <v>41</v>
+      </c>
+      <c r="CG6" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="CH6" s="30">
+        <v>1</v>
+      </c>
+      <c r="CI6" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ6" s="30">
+        <v>2</v>
+      </c>
+      <c r="CK6" s="30">
+        <v>11</v>
+      </c>
+      <c r="CL6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN6" s="35">
+        <v>2</v>
+      </c>
+      <c r="CO6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS6" s="30">
+        <v>8</v>
+      </c>
+      <c r="CT6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV6" s="30">
+        <v>230</v>
+      </c>
+      <c r="CW6" s="30">
+        <v>4</v>
+      </c>
+      <c r="CX6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY6" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ6" s="30">
+        <v>2</v>
+      </c>
+      <c r="DA6" s="30">
+        <v>12</v>
+      </c>
+      <c r="DB6" s="30"/>
+      <c r="DC6" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD6" s="30">
+        <v>13</v>
+      </c>
+      <c r="DE6" s="30">
+        <v>5</v>
+      </c>
+      <c r="DF6" s="7">
+        <f>SUM(CI6:DE6)</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2369,8 +2979,88 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH7" t="s">
+        <v>42</v>
+      </c>
+      <c r="CG7" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="CH7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP7" s="30">
+        <v>4</v>
+      </c>
+      <c r="CQ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW7" s="30">
+        <v>51</v>
+      </c>
+      <c r="CX7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY7" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA7" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB7" s="30"/>
+      <c r="DC7" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD7" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE7" s="30">
+        <v>1</v>
+      </c>
+      <c r="DF7" s="7">
+        <f>SUM(CI7:DE7)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2532,8 +3222,88 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH8" t="s">
+        <v>43</v>
+      </c>
+      <c r="CG8" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="CH8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN8" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX8" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY8" s="30">
+        <v>9</v>
+      </c>
+      <c r="CZ8" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA8" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB8" s="30"/>
+      <c r="DC8" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD8" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF8" s="7">
+        <f>SUM(CI8:DE8)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2695,8 +3465,88 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH9" t="s">
+        <v>23</v>
+      </c>
+      <c r="CG9" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="CH9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN9" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX9" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY9" s="30">
+        <v>2</v>
+      </c>
+      <c r="CZ9" s="30">
+        <v>2</v>
+      </c>
+      <c r="DA9" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB9" s="30"/>
+      <c r="DC9" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD9" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE9" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF9" s="7">
+        <f>SUM(CI9:DE9)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2858,8 +3708,88 @@
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-    </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH10" t="s">
+        <v>4</v>
+      </c>
+      <c r="CG10" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="CH10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN10" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="30">
+        <v>113</v>
+      </c>
+      <c r="CR10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY10" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ10" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA10" s="30">
+        <v>4</v>
+      </c>
+      <c r="DB10" s="30"/>
+      <c r="DC10" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD10" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE10" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF10" s="7">
+        <f>SUM(CI10:DE10)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3021,8 +3951,88 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH11" t="s">
+        <v>44</v>
+      </c>
+      <c r="CG11" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="CH11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI11" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK11" s="30">
+        <v>2</v>
+      </c>
+      <c r="CL11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN11" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO11" s="30">
+        <v>2</v>
+      </c>
+      <c r="CP11" s="30">
+        <v>20</v>
+      </c>
+      <c r="CQ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV11" s="30">
+        <v>3</v>
+      </c>
+      <c r="CW11" s="30">
+        <v>10</v>
+      </c>
+      <c r="CX11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY11" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA11" s="30">
+        <v>1</v>
+      </c>
+      <c r="DB11" s="30"/>
+      <c r="DC11" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD11" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE11" s="30">
+        <v>8</v>
+      </c>
+      <c r="DF11" s="7">
+        <f>SUM(CI11:DE11)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3184,8 +4194,88 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH12" t="s">
+        <v>45</v>
+      </c>
+      <c r="CG12" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="CH12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI12" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN12" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO12" s="30">
+        <v>2</v>
+      </c>
+      <c r="CP12" s="30">
+        <v>2</v>
+      </c>
+      <c r="CQ12" s="30">
+        <v>2</v>
+      </c>
+      <c r="CR12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS12" s="30">
+        <v>2</v>
+      </c>
+      <c r="CT12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY12" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ12" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA12" s="30">
+        <v>46</v>
+      </c>
+      <c r="DB12" s="30"/>
+      <c r="DC12" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD12" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE12" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF12" s="7">
+        <f>SUM(CI12:DE12)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3347,8 +4437,88 @@
         <f t="shared" si="1"/>
         <v>254</v>
       </c>
-    </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH13" t="s">
+        <v>46</v>
+      </c>
+      <c r="CG13" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="CH13" s="30">
+        <v>1</v>
+      </c>
+      <c r="CI13" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ13" s="30">
+        <v>3</v>
+      </c>
+      <c r="CK13" s="30">
+        <v>2</v>
+      </c>
+      <c r="CL13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN13" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO13" s="30">
+        <v>1</v>
+      </c>
+      <c r="CP13" s="30">
+        <v>247</v>
+      </c>
+      <c r="CQ13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY13" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ13" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA13" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB13" s="30"/>
+      <c r="DC13" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD13" s="30">
+        <v>0</v>
+      </c>
+      <c r="DE13" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF13" s="7">
+        <f>SUM(CI13:DE13)</f>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3510,8 +4680,88 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH14" t="s">
+        <v>47</v>
+      </c>
+      <c r="CG14" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="CH14" s="30">
+        <v>8</v>
+      </c>
+      <c r="CI14" s="34">
+        <v>3</v>
+      </c>
+      <c r="CJ14" s="30">
+        <v>1</v>
+      </c>
+      <c r="CK14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN14" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS14" s="30">
+        <v>4</v>
+      </c>
+      <c r="CT14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU14" s="30">
+        <v>1</v>
+      </c>
+      <c r="CV14" s="30">
+        <v>1</v>
+      </c>
+      <c r="CW14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX14" s="30">
+        <v>3</v>
+      </c>
+      <c r="CY14" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ14" s="30">
+        <v>1</v>
+      </c>
+      <c r="DA14" s="30">
+        <v>2</v>
+      </c>
+      <c r="DB14" s="30"/>
+      <c r="DC14" s="30">
+        <v>1</v>
+      </c>
+      <c r="DD14" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE14" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF14" s="7">
+        <f>SUM(CI14:DE14)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3673,8 +4923,88 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH15" t="s">
+        <v>48</v>
+      </c>
+      <c r="CG15" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="CH15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI15" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN15" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS15" s="30">
+        <v>1</v>
+      </c>
+      <c r="CT15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY15" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ15" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA15" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB15" s="30"/>
+      <c r="DC15" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD15" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE15" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF15" s="7">
+        <f>SUM(CI15:DE15)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3836,8 +5166,88 @@
         <f t="shared" si="1"/>
         <v>708</v>
       </c>
-    </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH16" t="s">
+        <v>49</v>
+      </c>
+      <c r="CG16" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH16" s="30">
+        <v>25</v>
+      </c>
+      <c r="CI16" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ16" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK16" s="30">
+        <v>19</v>
+      </c>
+      <c r="CL16" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM16" s="30">
+        <v>1</v>
+      </c>
+      <c r="CN16" s="35">
+        <v>1</v>
+      </c>
+      <c r="CO16" s="30">
+        <v>60</v>
+      </c>
+      <c r="CP16" s="30">
+        <v>110</v>
+      </c>
+      <c r="CQ16" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR16" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS16" s="30">
+        <v>35</v>
+      </c>
+      <c r="CT16" s="30">
+        <v>7</v>
+      </c>
+      <c r="CU16" s="30">
+        <v>4</v>
+      </c>
+      <c r="CV16" s="30">
+        <v>8</v>
+      </c>
+      <c r="CW16" s="30">
+        <v>4</v>
+      </c>
+      <c r="CX16" s="30">
+        <v>1</v>
+      </c>
+      <c r="CY16" s="30">
+        <v>5</v>
+      </c>
+      <c r="CZ16" s="30">
+        <v>9</v>
+      </c>
+      <c r="DA16" s="30">
+        <v>143</v>
+      </c>
+      <c r="DB16" s="30"/>
+      <c r="DC16" s="30">
+        <v>1</v>
+      </c>
+      <c r="DD16" s="30">
+        <v>260</v>
+      </c>
+      <c r="DE16" s="30">
+        <v>15</v>
+      </c>
+      <c r="DF16" s="7">
+        <f>SUM(CI16:DE16)</f>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3999,8 +5409,88 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH17" t="s">
+        <v>50</v>
+      </c>
+      <c r="CG17" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CI17" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN17" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO17" s="30">
+        <v>4</v>
+      </c>
+      <c r="CP17" s="30">
+        <v>7</v>
+      </c>
+      <c r="CQ17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR17" s="30">
+        <v>3</v>
+      </c>
+      <c r="CS17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CT17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX17" s="30">
+        <v>1</v>
+      </c>
+      <c r="CY17" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ17" s="30">
+        <v>2</v>
+      </c>
+      <c r="DA17" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB17" s="30"/>
+      <c r="DC17" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD17" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE17" s="30">
+        <v>6</v>
+      </c>
+      <c r="DF17" s="7">
+        <f>SUM(CI17:DE17)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4162,8 +5652,88 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH18" t="s">
+        <v>18</v>
+      </c>
+      <c r="CG18" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH18" s="30">
+        <v>10</v>
+      </c>
+      <c r="CI18" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ18" s="30">
+        <v>3</v>
+      </c>
+      <c r="CK18" s="30">
+        <v>1</v>
+      </c>
+      <c r="CL18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN18" s="35">
+        <v>15</v>
+      </c>
+      <c r="CO18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CS18" s="30">
+        <v>2</v>
+      </c>
+      <c r="CT18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY18" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ18" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA18" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB18" s="30"/>
+      <c r="DC18" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD18" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE18" s="30">
+        <v>0</v>
+      </c>
+      <c r="DF18" s="7">
+        <f>SUM(CI18:DE18)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4325,8 +5895,88 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BH19" t="s">
+        <v>51</v>
+      </c>
+      <c r="CG19" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="CH19" s="30">
+        <v>10</v>
+      </c>
+      <c r="CI19" s="34">
+        <v>0</v>
+      </c>
+      <c r="CJ19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CK19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CL19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CM19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CN19" s="35">
+        <v>0</v>
+      </c>
+      <c r="CO19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CP19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CQ19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CR19" s="30">
+        <v>1</v>
+      </c>
+      <c r="CS19" s="30">
+        <v>2</v>
+      </c>
+      <c r="CT19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CU19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CV19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CW19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CX19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CY19" s="30">
+        <v>0</v>
+      </c>
+      <c r="CZ19" s="30">
+        <v>0</v>
+      </c>
+      <c r="DA19" s="30">
+        <v>0</v>
+      </c>
+      <c r="DB19" s="30"/>
+      <c r="DC19" s="30">
+        <v>0</v>
+      </c>
+      <c r="DD19" s="30">
+        <v>1</v>
+      </c>
+      <c r="DE19" s="30">
+        <v>1</v>
+      </c>
+      <c r="DF19" s="7">
+        <f>SUM(CI19:DE19)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:110" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4488,8 +6138,88 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BH20" t="s">
+        <v>52</v>
+      </c>
+      <c r="CG20" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="CH20" s="37">
+        <v>13</v>
+      </c>
+      <c r="CI20" s="36">
+        <v>0</v>
+      </c>
+      <c r="CJ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CK20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CL20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CM20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CN20" s="38">
+        <v>1</v>
+      </c>
+      <c r="CO20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CP20" s="37">
+        <v>2</v>
+      </c>
+      <c r="CQ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CR20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CS20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CT20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CU20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CV20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CW20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CX20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CY20" s="37">
+        <v>0</v>
+      </c>
+      <c r="CZ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="DA20" s="37">
+        <v>0</v>
+      </c>
+      <c r="DB20" s="37"/>
+      <c r="DC20" s="37">
+        <v>0</v>
+      </c>
+      <c r="DD20" s="37">
+        <v>0</v>
+      </c>
+      <c r="DE20" s="37">
+        <v>0</v>
+      </c>
+      <c r="DF20" s="10">
+        <f>SUM(CI20:DE20)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:110" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4689,8 +6419,105 @@
         <f t="shared" si="1"/>
         <v>2080</v>
       </c>
-    </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH21" t="s">
+        <v>53</v>
+      </c>
+      <c r="CH21" s="9">
+        <f t="shared" ref="CH21" si="4">SUM(CH2:CH20)</f>
+        <v>86</v>
+      </c>
+      <c r="CI21" s="8">
+        <f>SUM(CI2:CI20)</f>
+        <v>7</v>
+      </c>
+      <c r="CJ21" s="9">
+        <f>SUM(CJ2:CJ20)</f>
+        <v>10</v>
+      </c>
+      <c r="CK21" s="9">
+        <f>SUM(CK2:CK20)</f>
+        <v>47</v>
+      </c>
+      <c r="CL21" s="9"/>
+      <c r="CM21" s="9">
+        <f>SUM(CM2:CM20)</f>
+        <v>3</v>
+      </c>
+      <c r="CN21" s="10">
+        <f>SUM(CN2:CN20)</f>
+        <v>24</v>
+      </c>
+      <c r="CO21" s="9">
+        <f>SUM(CO2:CO20)</f>
+        <v>71</v>
+      </c>
+      <c r="CP21" s="9">
+        <f>SUM(CP2:CP20)</f>
+        <v>398</v>
+      </c>
+      <c r="CQ21" s="9">
+        <f>SUM(CQ2:CQ20)</f>
+        <v>115</v>
+      </c>
+      <c r="CR21" s="9">
+        <f>SUM(CR2:CR20)</f>
+        <v>4</v>
+      </c>
+      <c r="CS21" s="9">
+        <f t="shared" ref="CS21:DE21" si="5">SUM(CS2:CS20)</f>
+        <v>80</v>
+      </c>
+      <c r="CT21" s="9">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="CU21" s="9">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="CV21" s="9">
+        <f t="shared" si="5"/>
+        <v>261</v>
+      </c>
+      <c r="CW21" s="9">
+        <f t="shared" si="5"/>
+        <v>97</v>
+      </c>
+      <c r="CX21" s="9">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="CY21" s="9">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="CZ21" s="9">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="DA21" s="9">
+        <f t="shared" si="5"/>
+        <v>217</v>
+      </c>
+      <c r="DB21" s="9"/>
+      <c r="DC21" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="DD21" s="9">
+        <f t="shared" si="5"/>
+        <v>362</v>
+      </c>
+      <c r="DE21" s="9">
+        <f t="shared" si="5"/>
+        <v>59</v>
+      </c>
+      <c r="DF21" s="11">
+        <f>SUM(CI21:DE21)</f>
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4706,8 +6533,11 @@
       <c r="F22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4723,8 +6553,11 @@
       <c r="F23" s="45" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4738,8 +6571,11 @@
         <v>1</v>
       </c>
       <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4753,8 +6589,11 @@
         <v>8</v>
       </c>
       <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4769,7 +6608,7 @@
       </c>
       <c r="F26" s="28"/>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4784,7 +6623,7 @@
       </c>
       <c r="F27" s="28"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4799,7 +6638,7 @@
       </c>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4814,7 +6653,7 @@
       </c>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4829,7 +6668,7 @@
       </c>
       <c r="F30" s="28"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4844,7 +6683,7 @@
       </c>
       <c r="F31" s="28"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10665,6 +12504,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:AC20">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI2:BD20">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CI2:DE20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -10674,7 +12533,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:BD20">
+  <conditionalFormatting sqref="CH2:CH20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
he pasado a porcentaje la matriz de usos especificos y la he perarado para el Word
</commit_message>
<xml_diff>
--- a/Excel/matriz_tabla_contingencia.xlsx
+++ b/Excel/matriz_tabla_contingencia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="USOS_GENERAL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="43">
   <si>
     <t>Agrario</t>
   </si>
@@ -118,6 +118,42 @@
   </si>
   <si>
     <t>EN HUMEDAL</t>
+  </si>
+  <si>
+    <t>MUCVA  (%) / SIOSE (%)</t>
+  </si>
+  <si>
+    <t>Áreas agrarias heterogéneas</t>
+  </si>
+  <si>
+    <t>Áreas con fuertes procesos erosivos</t>
+  </si>
+  <si>
+    <t>Cultivos herbáceos</t>
+  </si>
+  <si>
+    <t>Leñoso regadío</t>
+  </si>
+  <si>
+    <t>Leñoso secano</t>
+  </si>
+  <si>
+    <t>Mares y océanos</t>
+  </si>
+  <si>
+    <t>Ríos, cauces o ramblas</t>
+  </si>
+  <si>
+    <t>Vegetación con eucaliptos</t>
+  </si>
+  <si>
+    <t>Vegetación natural</t>
+  </si>
+  <si>
+    <t>Vegetación riparia</t>
+  </si>
+  <si>
+    <t>Zonas en construcción</t>
   </si>
 </sst>
 </file>
@@ -344,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -400,6 +436,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:G16"/>
     </sheetView>
   </sheetViews>
@@ -1756,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW24"/>
+  <dimension ref="A1:AW25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24:AV24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL28" sqref="AL28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,526 +1837,360 @@
     <col min="16" max="17" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="48" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="199.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:49" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="R2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="S2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="U2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="W2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD1" s="28" t="s">
+      <c r="Z2" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA2" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AE2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AF2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AG2" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH2" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AK2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AL2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="AM1" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN1" s="28" t="s">
+      <c r="AM2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="28" t="s">
+      <c r="AO2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AP1" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR1" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="AS1" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT1" s="28" t="s">
+      <c r="AP2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR2" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS2" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AU1" s="28" t="s">
+      <c r="AU2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="AV1" s="29" t="s">
+      <c r="AV2" s="39" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3">
-        <v>42</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3">
-        <v>36</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>23</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>6</v>
-      </c>
-      <c r="P2" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3">
-        <v>36</v>
-      </c>
-      <c r="S2" s="3">
-        <v>13</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0</v>
-      </c>
-      <c r="X2" s="4">
-        <f>SUM(B2:W2)</f>
-        <v>180</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="5">
-        <f>B2/$AW$24</f>
-        <v>9.6153846153846159E-4</v>
-      </c>
-      <c r="AB2" s="1">
-        <f t="shared" ref="AB2:AV2" si="0">C2/$AW$24</f>
-        <v>2.403846153846154E-3</v>
-      </c>
-      <c r="AC2" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0192307692307693E-2</v>
-      </c>
-      <c r="AD2" s="1">
-        <f t="shared" si="0"/>
-        <v>1.4423076923076924E-3</v>
-      </c>
-      <c r="AE2" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9230769230769232E-3</v>
-      </c>
-      <c r="AF2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG2" s="1">
-        <f t="shared" si="0"/>
-        <v>3.3653846153846156E-3</v>
-      </c>
-      <c r="AH2" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7307692307692309E-2</v>
-      </c>
-      <c r="AI2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1057692307692308E-2</v>
-      </c>
-      <c r="AL2" s="1">
-        <f t="shared" si="0"/>
-        <v>4.807692307692308E-4</v>
-      </c>
-      <c r="AM2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8846153846153848E-3</v>
-      </c>
-      <c r="AO2" s="1">
-        <f t="shared" si="0"/>
-        <v>9.6153846153846159E-4</v>
-      </c>
-      <c r="AP2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7307692307692309E-2</v>
-      </c>
-      <c r="AR2" s="1">
-        <f t="shared" si="0"/>
-        <v>6.2500000000000003E-3</v>
-      </c>
-      <c r="AS2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AT2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AU2" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AV2" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AW2" s="4">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>23</v>
+      </c>
+      <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="6">
-        <v>0</v>
-      </c>
-      <c r="X3" s="6">
-        <f t="shared" ref="X3:X23" si="1">SUM(B3:W3)</f>
-        <v>4</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>21</v>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>6</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>36</v>
+      </c>
+      <c r="S3" s="3">
+        <v>13</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <f>SUM(B3:W3)</f>
+        <v>180</v>
+      </c>
+      <c r="Z3" s="41" t="s">
+        <v>32</v>
       </c>
       <c r="AA3" s="5">
-        <f t="shared" ref="AA3:AA23" si="2">B3/$AW$24</f>
-        <v>0</v>
+        <f>B3/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AB3" s="1">
-        <f t="shared" ref="AB3:AB23" si="3">C3/$AW$24</f>
-        <v>9.6153846153846159E-4</v>
+        <f t="shared" ref="AB3:AV3" si="0">C3/$X$25*100</f>
+        <v>0.24038461538461539</v>
       </c>
       <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC23" si="4">D3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.0192307692307692</v>
       </c>
       <c r="AD3" s="1">
-        <f t="shared" ref="AD3:AD23" si="5">E3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AE3" s="1">
-        <f t="shared" ref="AE3:AE23" si="6">F3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AF3" s="1">
-        <f t="shared" ref="AF3:AF23" si="7">G3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <f t="shared" ref="AG3:AG23" si="8">H3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33653846153846156</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" ref="AH3:AH23" si="9">I3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.7307692307692308</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" ref="AI3:AI23" si="10">J3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <f t="shared" ref="AJ3:AJ23" si="11">K3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK3" s="1">
-        <f t="shared" ref="AK3:AK23" si="12">L3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.1057692307692308</v>
       </c>
       <c r="AL3" s="1">
-        <f t="shared" ref="AL3:AL23" si="13">M3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AM3" s="1">
-        <f t="shared" ref="AM3:AM23" si="14">N3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AN3" s="1">
-        <f t="shared" ref="AN3:AN23" si="15">O3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.28846153846153849</v>
       </c>
       <c r="AO3" s="1">
-        <f t="shared" ref="AO3:AO23" si="16">P3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AP3" s="1">
-        <f t="shared" ref="AP3:AP23" si="17">Q3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AQ3" s="1">
-        <f t="shared" ref="AQ3:AQ23" si="18">R3/$AW$24</f>
-        <v>4.807692307692308E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.7307692307692308</v>
       </c>
       <c r="AR3" s="1">
-        <f t="shared" ref="AR3:AR23" si="19">S3/$AW$24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.625</v>
       </c>
       <c r="AS3" s="1">
-        <f t="shared" ref="AS3:AS23" si="20">T3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AT3" s="1">
-        <f t="shared" ref="AT3:AT23" si="21">U3/$AW$24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AU3" s="1">
-        <f t="shared" ref="AU3:AU23" si="22">V3/$AW$24</f>
-        <v>4.807692307692308E-4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="AV3" s="6">
-        <f t="shared" ref="AV3:AV23" si="23">W3/$AW$24</f>
-        <v>0</v>
-      </c>
-      <c r="AW3" s="6">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AW3" s="45">
+        <f>SUM(AA3:AV3)</f>
+        <v>8.6538461538461533</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>18</v>
-      </c>
       <c r="D4" s="1">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -2303,236 +2199,237 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="S4" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <v>1</v>
       </c>
       <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" ref="X4:X24" si="1">SUM(B4:W4)</f>
         <v>4</v>
       </c>
-      <c r="X4" s="6">
-        <f t="shared" si="1"/>
-        <v>240</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>17</v>
+      <c r="Z4" s="42" t="s">
+        <v>33</v>
       </c>
       <c r="AA4" s="5">
-        <f t="shared" si="2"/>
-        <v>9.6153846153846159E-4</v>
+        <f t="shared" ref="AA4:AA24" si="2">B4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AB4" s="1">
-        <f t="shared" si="3"/>
-        <v>8.6538461538461543E-3</v>
+        <f t="shared" ref="AB4:AB24" si="3">C4/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AC4" s="1">
-        <f t="shared" si="4"/>
-        <v>2.7403846153846154E-2</v>
+        <f t="shared" ref="AC4:AC24" si="4">D4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AD4" s="1">
-        <f t="shared" si="5"/>
-        <v>4.3269230769230772E-3</v>
+        <f t="shared" ref="AD4:AD24" si="5">E4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AE4" s="1">
-        <f t="shared" si="6"/>
-        <v>7.2115384615384619E-3</v>
+        <f t="shared" ref="AE4:AE24" si="6">F4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AF4" s="1">
-        <f t="shared" si="7"/>
-        <v>1.3461538461538462E-2</v>
+        <f t="shared" ref="AF4:AF24" si="7">G4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AG4" s="1">
-        <f t="shared" si="8"/>
-        <v>1.4423076923076924E-3</v>
+        <f t="shared" ref="AG4:AG24" si="8">H4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="9"/>
-        <v>5.2884615384615388E-3</v>
+        <f t="shared" ref="AH4:AH24" si="9">I4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="AI4:AI24" si="10">J4/$X$25*100</f>
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
-        <f t="shared" si="11"/>
-        <v>9.6153846153846159E-4</v>
+        <f t="shared" ref="AJ4:AJ24" si="11">K4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AK4" s="1">
-        <f t="shared" si="12"/>
-        <v>4.3269230769230772E-3</v>
+        <f t="shared" ref="AK4:AK24" si="12">L4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
-        <f t="shared" si="13"/>
-        <v>3.8461538461538464E-3</v>
+        <f t="shared" ref="AL4:AL24" si="13">M4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AM4" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="AM4:AM24" si="14">N4/$X$25*100</f>
         <v>0</v>
       </c>
       <c r="AN4" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="AN4:AN24" si="15">O4/$X$25*100</f>
         <v>0</v>
       </c>
       <c r="AO4" s="1">
-        <f t="shared" si="16"/>
-        <v>7.6923076923076927E-3</v>
+        <f t="shared" ref="AO4:AO24" si="16">P4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AP4" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="AP4:AP24" si="17">Q4/$X$25*100</f>
         <v>0</v>
       </c>
       <c r="AQ4" s="1">
-        <f t="shared" si="18"/>
-        <v>2.2115384615384617E-2</v>
+        <f t="shared" ref="AQ4:AQ24" si="18">R4/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR4" s="1">
-        <f t="shared" si="19"/>
-        <v>4.807692307692308E-3</v>
+        <f t="shared" ref="AR4:AR24" si="19">S4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AS4" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="AS4:AS24" si="20">T4/$X$25*100</f>
         <v>0</v>
       </c>
       <c r="AT4" s="1">
-        <f t="shared" si="21"/>
-        <v>4.807692307692308E-4</v>
+        <f t="shared" ref="AT4:AT24" si="21">U4/$X$25*100</f>
+        <v>0</v>
       </c>
       <c r="AU4" s="1">
-        <f t="shared" si="22"/>
-        <v>4.807692307692308E-4</v>
+        <f t="shared" ref="AU4:AU24" si="22">V4/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AV4" s="6">
-        <f t="shared" si="23"/>
-        <v>1.9230769230769232E-3</v>
-      </c>
-      <c r="AW4" s="6">
-        <v>240</v>
+        <f t="shared" ref="AV4:AV24" si="23">W4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="AW4" s="46">
+        <f t="shared" ref="AW4:AW24" si="24">SUM(AA4:AV4)</f>
+        <v>0.19230769230769232</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="F5" s="1">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>46</v>
+      </c>
+      <c r="S5" s="1">
+        <v>10</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X5" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>9</v>
+        <v>240</v>
+      </c>
+      <c r="Z5" s="42" t="s">
+        <v>34</v>
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AB5" s="1">
         <f t="shared" si="3"/>
-        <v>4.807692307692308E-4</v>
+        <v>0.86538461538461542</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.7403846153846154</v>
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.43269230769230771</v>
       </c>
       <c r="AE5" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.72115384615384615</v>
       </c>
       <c r="AF5" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.3461538461538463</v>
       </c>
       <c r="AG5" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AH5" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.52884615384615385</v>
       </c>
       <c r="AI5" s="1">
         <f t="shared" si="10"/>
@@ -2540,15 +2437,15 @@
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AK5" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.43269230769230771</v>
       </c>
       <c r="AL5" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AM5" s="1">
         <f t="shared" si="14"/>
@@ -2560,7 +2457,7 @@
       </c>
       <c r="AO5" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="AP5" s="1">
         <f t="shared" si="17"/>
@@ -2568,11 +2465,11 @@
       </c>
       <c r="AQ5" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2.2115384615384617</v>
       </c>
       <c r="AR5" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.48076923076923078</v>
       </c>
       <c r="AS5" s="1">
         <f t="shared" si="20"/>
@@ -2580,41 +2477,42 @@
       </c>
       <c r="AT5" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AU5" s="1">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AV5" s="6">
         <f t="shared" si="23"/>
-        <v>4.807692307692308E-4</v>
-      </c>
-      <c r="AW5" s="6">
-        <v>2</v>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="AW5" s="46">
+        <f t="shared" si="24"/>
+        <v>11.538461538461538</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -2629,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
@@ -2641,35 +2539,35 @@
         <v>0</v>
       </c>
       <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="6">
         <v>1</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
-        <v>13</v>
-      </c>
-      <c r="S6" s="1">
-        <v>5</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1">
-        <v>2</v>
-      </c>
-      <c r="V6" s="1">
-        <v>0</v>
-      </c>
-      <c r="W6" s="6">
-        <v>2</v>
       </c>
       <c r="X6" s="6">
         <f t="shared" si="1"/>
-        <v>290</v>
-      </c>
-      <c r="Z6" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="Z6" s="42" t="s">
+        <v>9</v>
       </c>
       <c r="AA6" s="5">
         <f t="shared" si="2"/>
@@ -2677,7 +2575,7 @@
       </c>
       <c r="AB6" s="1">
         <f t="shared" si="3"/>
-        <v>3.8461538461538464E-3</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" si="4"/>
@@ -2685,15 +2583,15 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="5"/>
-        <v>5.2884615384615388E-3</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="1">
         <f t="shared" si="6"/>
-        <v>0.11057692307692307</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="1">
         <f t="shared" si="7"/>
-        <v>1.9230769230769232E-3</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="8"/>
@@ -2713,11 +2611,11 @@
       </c>
       <c r="AK6" s="1">
         <f t="shared" si="12"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="1">
         <f t="shared" si="13"/>
-        <v>5.7692307692307696E-3</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="1">
         <f t="shared" si="14"/>
@@ -2729,7 +2627,7 @@
       </c>
       <c r="AO6" s="1">
         <f t="shared" si="16"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="1">
         <f t="shared" si="17"/>
@@ -2737,11 +2635,11 @@
       </c>
       <c r="AQ6" s="1">
         <f t="shared" si="18"/>
-        <v>6.2500000000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="1">
         <f t="shared" si="19"/>
-        <v>2.403846153846154E-3</v>
+        <v>0</v>
       </c>
       <c r="AS6" s="1">
         <f t="shared" si="20"/>
@@ -2749,7 +2647,7 @@
       </c>
       <c r="AT6" s="1">
         <f t="shared" si="21"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="1">
         <f t="shared" si="22"/>
@@ -2757,33 +2655,34 @@
       </c>
       <c r="AV6" s="6">
         <f t="shared" si="23"/>
-        <v>9.6153846153846159E-4</v>
-      </c>
-      <c r="AW6" s="6">
-        <v>290</v>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="AW6" s="46">
+        <f t="shared" si="24"/>
+        <v>9.6153846153846159E-2</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="G7" s="1">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -2798,47 +2697,47 @@
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="S7" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
       </c>
       <c r="W7" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X7" s="6">
         <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>15</v>
+        <v>290</v>
+      </c>
+      <c r="Z7" s="42" t="s">
+        <v>5</v>
       </c>
       <c r="AA7" s="5">
         <f t="shared" si="2"/>
@@ -2846,7 +2745,7 @@
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="4"/>
@@ -2854,15 +2753,15 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.52884615384615385</v>
       </c>
       <c r="AE7" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>11.057692307692307</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="7"/>
-        <v>2.4519230769230769E-2</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="8"/>
@@ -2882,11 +2781,11 @@
       </c>
       <c r="AK7" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AL7" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.57692307692307698</v>
       </c>
       <c r="AM7" s="1">
         <f t="shared" si="14"/>
@@ -2894,11 +2793,11 @@
       </c>
       <c r="AN7" s="1">
         <f t="shared" si="15"/>
-        <v>1.9230769230769232E-3</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AP7" s="1">
         <f t="shared" si="17"/>
@@ -2906,11 +2805,11 @@
       </c>
       <c r="AQ7" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="AR7" s="1">
         <f t="shared" si="19"/>
-        <v>4.807692307692308E-4</v>
+        <v>0.24038461538461539</v>
       </c>
       <c r="AS7" s="1">
         <f t="shared" si="20"/>
@@ -2918,7 +2817,7 @@
       </c>
       <c r="AT7" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AU7" s="1">
         <f t="shared" si="22"/>
@@ -2926,15 +2825,16 @@
       </c>
       <c r="AV7" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="AW7" s="6">
-        <v>56</v>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="AW7" s="46">
+        <f t="shared" si="24"/>
+        <v>13.942307692307692</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -2952,13 +2852,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -2976,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -2988,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="1">
         <v>0</v>
@@ -3004,10 +2904,10 @@
       </c>
       <c r="X8" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>23</v>
+        <v>56</v>
+      </c>
+      <c r="Z8" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="AA8" s="5">
         <f t="shared" si="2"/>
@@ -3031,7 +2931,7 @@
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.4519230769230771</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="8"/>
@@ -3039,7 +2939,7 @@
       </c>
       <c r="AH8" s="1">
         <f t="shared" si="9"/>
-        <v>4.3269230769230772E-3</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="1">
         <f t="shared" si="10"/>
@@ -3063,7 +2963,7 @@
       </c>
       <c r="AN8" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AO8" s="1">
         <f t="shared" si="16"/>
@@ -3079,7 +2979,7 @@
       </c>
       <c r="AR8" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AS8" s="1">
         <f t="shared" si="20"/>
@@ -3097,13 +2997,14 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW8" s="6">
-        <v>9</v>
+      <c r="AW8" s="46">
+        <f t="shared" si="24"/>
+        <v>2.6923076923076925</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -3127,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -3136,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -3154,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -3173,10 +3074,10 @@
       </c>
       <c r="X9" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="Z9" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="AA9" s="5">
         <f t="shared" si="2"/>
@@ -3208,7 +3109,7 @@
       </c>
       <c r="AH9" s="1">
         <f t="shared" si="9"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0.43269230769230771</v>
       </c>
       <c r="AI9" s="1">
         <f t="shared" si="10"/>
@@ -3220,7 +3121,7 @@
       </c>
       <c r="AK9" s="1">
         <f t="shared" si="12"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AL9" s="1">
         <f t="shared" si="13"/>
@@ -3244,7 +3145,7 @@
       </c>
       <c r="AQ9" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AR9" s="1">
         <f t="shared" si="19"/>
@@ -3266,13 +3167,14 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW9" s="6">
-        <v>5</v>
+      <c r="AW9" s="46">
+        <f t="shared" si="24"/>
+        <v>0.43269230769230771</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -3296,19 +3198,19 @@
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
       </c>
       <c r="L10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -3323,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -3342,10 +3244,10 @@
       </c>
       <c r="X10" s="6">
         <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="Z10" s="42" t="s">
+        <v>36</v>
       </c>
       <c r="AA10" s="5">
         <f t="shared" si="2"/>
@@ -3377,11 +3279,11 @@
       </c>
       <c r="AH10" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AI10" s="1">
         <f t="shared" si="10"/>
-        <v>5.3846153846153849E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ10" s="1">
         <f t="shared" si="11"/>
@@ -3389,11 +3291,11 @@
       </c>
       <c r="AK10" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AL10" s="1">
         <f t="shared" si="13"/>
-        <v>2.8846153846153848E-3</v>
+        <v>0</v>
       </c>
       <c r="AM10" s="1">
         <f t="shared" si="14"/>
@@ -3413,7 +3315,7 @@
       </c>
       <c r="AQ10" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR10" s="1">
         <f t="shared" si="19"/>
@@ -3435,55 +3337,56 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW10" s="6">
-        <v>118</v>
+      <c r="AW10" s="46">
+        <f t="shared" si="24"/>
+        <v>0.24038461538461539</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>112</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>6</v>
       </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>2</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>2</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
       <c r="N11" s="1">
         <v>0</v>
       </c>
       <c r="O11" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
@@ -3495,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T11" s="1">
         <v>0</v>
@@ -3511,10 +3414,10 @@
       </c>
       <c r="X11" s="6">
         <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="Z11" s="5" t="s">
-        <v>6</v>
+        <v>118</v>
+      </c>
+      <c r="Z11" s="42" t="s">
+        <v>37</v>
       </c>
       <c r="AA11" s="5">
         <f t="shared" si="2"/>
@@ -3530,15 +3433,15 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="5"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="1">
         <f t="shared" si="6"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="7"/>
-        <v>4.807692307692308E-3</v>
+        <v>0</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="8"/>
@@ -3550,11 +3453,11 @@
       </c>
       <c r="AI11" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5.384615384615385</v>
       </c>
       <c r="AJ11" s="1">
         <f t="shared" si="11"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AK11" s="1">
         <f t="shared" si="12"/>
@@ -3562,7 +3465,7 @@
       </c>
       <c r="AL11" s="1">
         <f t="shared" si="13"/>
-        <v>4.807692307692308E-4</v>
+        <v>0.28846153846153849</v>
       </c>
       <c r="AM11" s="1">
         <f t="shared" si="14"/>
@@ -3570,7 +3473,7 @@
       </c>
       <c r="AN11" s="1">
         <f t="shared" si="15"/>
-        <v>9.6153846153846159E-3</v>
+        <v>0</v>
       </c>
       <c r="AO11" s="1">
         <f t="shared" si="16"/>
@@ -3586,7 +3489,7 @@
       </c>
       <c r="AR11" s="1">
         <f t="shared" si="19"/>
-        <v>3.8461538461538464E-3</v>
+        <v>0</v>
       </c>
       <c r="AS11" s="1">
         <f t="shared" si="20"/>
@@ -3604,13 +3507,14 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW11" s="6">
-        <v>46</v>
+      <c r="AW11" s="46">
+        <f t="shared" si="24"/>
+        <v>5.6730769230769234</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -3622,13 +3526,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -3640,19 +3544,19 @@
         <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
@@ -3664,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
@@ -3680,10 +3584,10 @@
       </c>
       <c r="X12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="Z12" s="42" t="s">
+        <v>6</v>
       </c>
       <c r="AA12" s="5">
         <f t="shared" si="2"/>
@@ -3699,15 +3603,15 @@
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AE12" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AF12" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.48076923076923078</v>
       </c>
       <c r="AG12" s="1">
         <f t="shared" si="8"/>
@@ -3723,7 +3627,7 @@
       </c>
       <c r="AJ12" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AK12" s="1">
         <f t="shared" si="12"/>
@@ -3731,7 +3635,7 @@
       </c>
       <c r="AL12" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AM12" s="1">
         <f t="shared" si="14"/>
@@ -3739,7 +3643,7 @@
       </c>
       <c r="AN12" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.96153846153846156</v>
       </c>
       <c r="AO12" s="1">
         <f t="shared" si="16"/>
@@ -3755,7 +3659,7 @@
       </c>
       <c r="AR12" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AS12" s="1">
         <f t="shared" si="20"/>
@@ -3773,19 +3677,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW12" s="6">
-        <v>0</v>
+      <c r="AW12" s="46">
+        <f t="shared" si="24"/>
+        <v>2.2115384615384617</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -3806,22 +3711,22 @@
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1">
         <v>0</v>
@@ -3849,10 +3754,10 @@
       </c>
       <c r="X13" s="6">
         <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="42" t="s">
+        <v>16</v>
       </c>
       <c r="AA13" s="5">
         <f t="shared" si="2"/>
@@ -3860,7 +3765,7 @@
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="3"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="4"/>
@@ -3888,11 +3793,11 @@
       </c>
       <c r="AI13" s="1">
         <f t="shared" si="10"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="1">
         <f t="shared" si="11"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AK13" s="1">
         <f t="shared" si="12"/>
@@ -3900,7 +3805,7 @@
       </c>
       <c r="AL13" s="1">
         <f t="shared" si="13"/>
-        <v>2.1634615384615384E-2</v>
+        <v>0</v>
       </c>
       <c r="AM13" s="1">
         <f t="shared" si="14"/>
@@ -3908,7 +3813,7 @@
       </c>
       <c r="AN13" s="1">
         <f t="shared" si="15"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AO13" s="1">
         <f t="shared" si="16"/>
@@ -3942,19 +3847,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW13" s="6">
-        <v>53</v>
+      <c r="AW13" s="47">
+        <f t="shared" si="24"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -3975,22 +3881,22 @@
         <v>0</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14" s="1">
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -4018,10 +3924,10 @@
       </c>
       <c r="X14" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="5" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+      <c r="Z14" s="42" t="s">
+        <v>20</v>
       </c>
       <c r="AA14" s="5">
         <f t="shared" si="2"/>
@@ -4029,7 +3935,7 @@
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="4"/>
@@ -4057,11 +3963,11 @@
       </c>
       <c r="AI14" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AJ14" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AK14" s="1">
         <f t="shared" si="12"/>
@@ -4069,7 +3975,7 @@
       </c>
       <c r="AL14" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2.1634615384615383</v>
       </c>
       <c r="AM14" s="1">
         <f t="shared" si="14"/>
@@ -4077,7 +3983,7 @@
       </c>
       <c r="AN14" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AO14" s="1">
         <f t="shared" si="16"/>
@@ -4111,13 +4017,14 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW14" s="6">
-        <v>0</v>
+      <c r="AW14" s="46">
+        <f t="shared" si="24"/>
+        <v>2.5480769230769229</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -4129,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -4147,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <v>0</v>
@@ -4159,10 +4066,10 @@
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1">
         <v>0</v>
@@ -4177,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="U15" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V15" s="1">
         <v>0</v>
@@ -4187,10 +4094,10 @@
       </c>
       <c r="X15" s="6">
         <f t="shared" si="1"/>
-        <v>254</v>
-      </c>
-      <c r="Z15" s="5" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="42" t="s">
+        <v>38</v>
       </c>
       <c r="AA15" s="5">
         <f t="shared" si="2"/>
@@ -4206,7 +4113,7 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="5"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="1">
         <f t="shared" si="6"/>
@@ -4230,7 +4137,7 @@
       </c>
       <c r="AJ15" s="1">
         <f t="shared" si="11"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AK15" s="1">
         <f t="shared" si="12"/>
@@ -4246,11 +4153,11 @@
       </c>
       <c r="AN15" s="1">
         <f t="shared" si="15"/>
-        <v>0.11874999999999999</v>
+        <v>0</v>
       </c>
       <c r="AO15" s="1">
         <f t="shared" si="16"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AP15" s="1">
         <f t="shared" si="17"/>
@@ -4270,7 +4177,7 @@
       </c>
       <c r="AT15" s="1">
         <f t="shared" si="21"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AU15" s="1">
         <f t="shared" si="22"/>
@@ -4280,73 +4187,74 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW15" s="6">
-        <v>254</v>
+      <c r="AW15" s="47">
+        <f t="shared" si="24"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>247</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
         <v>3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1">
-        <v>2</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>8</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-      <c r="T16" s="1">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1">
-        <v>1</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
@@ -4356,30 +4264,30 @@
       </c>
       <c r="X16" s="6">
         <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>7</v>
+        <v>254</v>
+      </c>
+      <c r="Z16" s="42" t="s">
+        <v>4</v>
       </c>
       <c r="AA16" s="5">
         <f t="shared" si="2"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="3"/>
-        <v>1.9230769230769232E-3</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="4"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AE16" s="1">
         <f t="shared" si="6"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="1">
         <f t="shared" si="7"/>
@@ -4387,7 +4295,7 @@
       </c>
       <c r="AG16" s="1">
         <f t="shared" si="8"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="1">
         <f t="shared" si="9"/>
@@ -4399,15 +4307,15 @@
       </c>
       <c r="AJ16" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AK16" s="1">
         <f t="shared" si="12"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="1">
         <f t="shared" si="13"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AM16" s="1">
         <f t="shared" si="14"/>
@@ -4415,19 +4323,19 @@
       </c>
       <c r="AN16" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>11.875</v>
       </c>
       <c r="AO16" s="1">
         <f t="shared" si="16"/>
-        <v>3.8461538461538464E-3</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AP16" s="1">
         <f t="shared" si="17"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AR16" s="1">
         <f t="shared" si="19"/>
@@ -4439,7 +4347,7 @@
       </c>
       <c r="AT16" s="1">
         <f t="shared" si="21"/>
-        <v>4.807692307692308E-4</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AU16" s="1">
         <f t="shared" si="22"/>
@@ -4449,34 +4357,35 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW16" s="6">
-        <v>26</v>
+      <c r="AW16" s="46">
+        <f t="shared" si="24"/>
+        <v>12.211538461538463</v>
       </c>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B17" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -4488,10 +4397,10 @@
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
@@ -4500,10 +4409,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="1">
         <v>1</v>
@@ -4515,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="1">
         <v>0</v>
@@ -4525,22 +4434,22 @@
       </c>
       <c r="X17" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="Z17" s="42" t="s">
+        <v>7</v>
       </c>
       <c r="AA17" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="3"/>
-        <v>4.807692307692308E-4</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AC17" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="5"/>
@@ -4548,7 +4457,7 @@
       </c>
       <c r="AE17" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AF17" s="1">
         <f t="shared" si="7"/>
@@ -4556,7 +4465,7 @@
       </c>
       <c r="AG17" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AH17" s="1">
         <f t="shared" si="9"/>
@@ -4572,11 +4481,11 @@
       </c>
       <c r="AK17" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AL17" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AM17" s="1">
         <f t="shared" si="14"/>
@@ -4588,15 +4497,15 @@
       </c>
       <c r="AO17" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AP17" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AQ17" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR17" s="1">
         <f t="shared" si="19"/>
@@ -4608,7 +4517,7 @@
       </c>
       <c r="AT17" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AU17" s="1">
         <f t="shared" si="22"/>
@@ -4618,67 +4527,68 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AW17" s="6">
-        <v>2</v>
+      <c r="AW17" s="46">
+        <f t="shared" si="24"/>
+        <v>1.2500000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="1">
-        <v>5</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
-        <v>60</v>
-      </c>
-      <c r="L18" s="1">
-        <v>9</v>
-      </c>
-      <c r="M18" s="1">
-        <v>143</v>
-      </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1">
-        <v>110</v>
-      </c>
-      <c r="P18" s="1">
-        <v>25</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>1</v>
-      </c>
-      <c r="R18" s="1">
-        <v>260</v>
-      </c>
       <c r="S18" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T18" s="1">
         <v>0</v>
@@ -4687,17 +4597,17 @@
         <v>0</v>
       </c>
       <c r="V18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X18" s="6">
         <f t="shared" si="1"/>
-        <v>708</v>
-      </c>
-      <c r="Z18" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="Z18" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="AA18" s="5">
         <f t="shared" si="2"/>
@@ -4705,31 +4615,31 @@
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="3"/>
-        <v>1.6826923076923076E-2</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AC18" s="1">
         <f t="shared" si="4"/>
-        <v>5.2884615384615388E-3</v>
+        <v>0</v>
       </c>
       <c r="AD18" s="1">
         <f t="shared" si="5"/>
-        <v>9.1346153846153851E-3</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="1">
         <f t="shared" si="6"/>
-        <v>3.8461538461538464E-3</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="1">
         <f t="shared" si="7"/>
-        <v>1.9230769230769232E-3</v>
+        <v>0</v>
       </c>
       <c r="AG18" s="1">
         <f t="shared" si="8"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="1">
         <f t="shared" si="9"/>
-        <v>2.403846153846154E-3</v>
+        <v>0</v>
       </c>
       <c r="AI18" s="1">
         <f t="shared" si="10"/>
@@ -4737,15 +4647,15 @@
       </c>
       <c r="AJ18" s="1">
         <f t="shared" si="11"/>
-        <v>2.8846153846153848E-2</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="1">
         <f t="shared" si="12"/>
-        <v>4.3269230769230772E-3</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="1">
         <f t="shared" si="13"/>
-        <v>6.8750000000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="AM18" s="1">
         <f t="shared" si="14"/>
@@ -4753,23 +4663,23 @@
       </c>
       <c r="AN18" s="1">
         <f t="shared" si="15"/>
-        <v>5.2884615384615384E-2</v>
+        <v>0</v>
       </c>
       <c r="AO18" s="1">
         <f t="shared" si="16"/>
-        <v>1.201923076923077E-2</v>
+        <v>0</v>
       </c>
       <c r="AP18" s="1">
         <f t="shared" si="17"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AQ18" s="1">
         <f t="shared" si="18"/>
-        <v>0.125</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR18" s="1">
         <f t="shared" si="19"/>
-        <v>7.2115384615384619E-3</v>
+        <v>0</v>
       </c>
       <c r="AS18" s="1">
         <f t="shared" si="20"/>
@@ -4781,92 +4691,93 @@
       </c>
       <c r="AU18" s="1">
         <f t="shared" si="22"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AV18" s="6">
         <f t="shared" si="23"/>
-        <v>4.807692307692308E-4</v>
-      </c>
-      <c r="AW18" s="6">
-        <v>708</v>
+        <v>0</v>
+      </c>
+      <c r="AW18" s="46">
+        <f t="shared" si="24"/>
+        <v>9.6153846153846159E-2</v>
       </c>
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="L19" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="N19" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O19" s="1">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="1">
+        <v>260</v>
+      </c>
+      <c r="S19" s="1">
+        <v>15</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
         <v>1</v>
       </c>
-      <c r="S19" s="1">
-        <v>6</v>
-      </c>
-      <c r="T19" s="1">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1">
-        <v>0</v>
-      </c>
-      <c r="V19" s="1">
-        <v>0</v>
-      </c>
       <c r="W19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="6">
         <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="Z19" s="5" t="s">
-        <v>14</v>
+        <v>708</v>
+      </c>
+      <c r="Z19" s="42" t="s">
+        <v>40</v>
       </c>
       <c r="AA19" s="5">
         <f t="shared" si="2"/>
@@ -4874,31 +4785,31 @@
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.6826923076923077</v>
       </c>
       <c r="AC19" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.52884615384615385</v>
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.91346153846153855</v>
       </c>
       <c r="AE19" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="AF19" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AG19" s="1">
         <f t="shared" si="8"/>
-        <v>4.807692307692308E-4</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AH19" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.24038461538461539</v>
       </c>
       <c r="AI19" s="1">
         <f t="shared" si="10"/>
@@ -4906,39 +4817,39 @@
       </c>
       <c r="AJ19" s="1">
         <f t="shared" si="11"/>
-        <v>1.9230769230769232E-3</v>
+        <v>2.8846153846153846</v>
       </c>
       <c r="AK19" s="1">
         <f t="shared" si="12"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0.43269230769230771</v>
       </c>
       <c r="AL19" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>6.8750000000000009</v>
       </c>
       <c r="AM19" s="1">
         <f t="shared" si="14"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="1">
         <f t="shared" si="15"/>
-        <v>3.3653846153846156E-3</v>
+        <v>5.2884615384615383</v>
       </c>
       <c r="AO19" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1.2019230769230771</v>
       </c>
       <c r="AP19" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AQ19" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>12.5</v>
       </c>
       <c r="AR19" s="1">
         <f t="shared" si="19"/>
-        <v>2.8846153846153848E-3</v>
+        <v>0.72115384615384615</v>
       </c>
       <c r="AS19" s="1">
         <f t="shared" si="20"/>
@@ -4950,64 +4861,65 @@
       </c>
       <c r="AU19" s="1">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AV19" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="AW19" s="6">
-        <v>24</v>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="AW19" s="46">
+        <f t="shared" si="24"/>
+        <v>34.038461538461533</v>
       </c>
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
       </c>
       <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>4</v>
+      </c>
+      <c r="L20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" s="1">
-        <v>0</v>
-      </c>
       <c r="M20" s="1">
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O20" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P20" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="1">
         <v>0</v>
@@ -5016,26 +4928,26 @@
         <v>1</v>
       </c>
       <c r="S20" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="X20" s="6">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="Z20" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="AA20" s="5">
         <f t="shared" si="2"/>
@@ -5043,7 +4955,7 @@
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="3"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="4"/>
@@ -5051,7 +4963,7 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="5"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="1">
         <f t="shared" si="6"/>
@@ -5063,7 +4975,7 @@
       </c>
       <c r="AG20" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AH20" s="1">
         <f t="shared" si="9"/>
@@ -5075,11 +4987,11 @@
       </c>
       <c r="AJ20" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="AK20" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AL20" s="1">
         <f t="shared" si="13"/>
@@ -5087,15 +4999,15 @@
       </c>
       <c r="AM20" s="1">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AN20" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.33653846153846156</v>
       </c>
       <c r="AO20" s="1">
         <f t="shared" si="16"/>
-        <v>4.807692307692308E-3</v>
+        <v>0</v>
       </c>
       <c r="AP20" s="1">
         <f t="shared" si="17"/>
@@ -5103,11 +5015,11 @@
       </c>
       <c r="AQ20" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR20" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.28846153846153849</v>
       </c>
       <c r="AS20" s="1">
         <f t="shared" si="20"/>
@@ -5115,7 +5027,7 @@
       </c>
       <c r="AT20" s="1">
         <f t="shared" si="21"/>
-        <v>1.4423076923076924E-3</v>
+        <v>0</v>
       </c>
       <c r="AU20" s="1">
         <f t="shared" si="22"/>
@@ -5123,15 +5035,16 @@
       </c>
       <c r="AV20" s="6">
         <f t="shared" si="23"/>
-        <v>7.2115384615384619E-3</v>
-      </c>
-      <c r="AW20" s="6">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="AW20" s="46">
+        <f t="shared" si="24"/>
+        <v>1.153846153846154</v>
       </c>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
@@ -5143,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -5170,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="1">
         <v>0</v>
@@ -5185,26 +5098,26 @@
         <v>1</v>
       </c>
       <c r="S21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21" s="6">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="X21" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="Z21" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="Z21" s="42" t="s">
+        <v>42</v>
       </c>
       <c r="AA21" s="5">
         <f t="shared" si="2"/>
@@ -5212,7 +5125,7 @@
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="3"/>
-        <v>9.6153846153846159E-4</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="4"/>
@@ -5220,7 +5133,7 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AE21" s="1">
         <f t="shared" si="6"/>
@@ -5256,7 +5169,7 @@
       </c>
       <c r="AM21" s="1">
         <f t="shared" si="14"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AN21" s="1">
         <f t="shared" si="15"/>
@@ -5264,7 +5177,7 @@
       </c>
       <c r="AO21" s="1">
         <f t="shared" si="16"/>
-        <v>4.807692307692308E-3</v>
+        <v>0.48076923076923078</v>
       </c>
       <c r="AP21" s="1">
         <f t="shared" si="17"/>
@@ -5272,11 +5185,11 @@
       </c>
       <c r="AQ21" s="1">
         <f t="shared" si="18"/>
-        <v>4.807692307692308E-4</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR21" s="1">
         <f t="shared" si="19"/>
-        <v>4.807692307692308E-4</v>
+        <v>0</v>
       </c>
       <c r="AS21" s="1">
         <f t="shared" si="20"/>
@@ -5284,7 +5197,7 @@
       </c>
       <c r="AT21" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>0.14423076923076925</v>
       </c>
       <c r="AU21" s="1">
         <f t="shared" si="22"/>
@@ -5292,69 +5205,70 @@
       </c>
       <c r="AV21" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="AW21" s="6">
-        <v>15</v>
+        <v>0.72115384615384615</v>
+      </c>
+      <c r="AW21" s="46">
+        <f t="shared" si="24"/>
+        <v>1.5384615384615385</v>
       </c>
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
         <v>10</v>
       </c>
-      <c r="B22" s="5">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>2</v>
-      </c>
-      <c r="P22" s="1">
-        <v>13</v>
-      </c>
       <c r="Q22" s="1">
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="1">
         <v>0</v>
@@ -5366,14 +5280,14 @@
         <v>0</v>
       </c>
       <c r="W22" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22" s="6">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="Z22" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="AA22" s="5">
         <f t="shared" si="2"/>
@@ -5381,7 +5295,7 @@
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.6153846153846159E-2</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="4"/>
@@ -5425,15 +5339,15 @@
       </c>
       <c r="AM22" s="1">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AN22" s="1">
         <f t="shared" si="15"/>
-        <v>9.6153846153846159E-4</v>
+        <v>0</v>
       </c>
       <c r="AO22" s="1">
         <f t="shared" si="16"/>
-        <v>6.2500000000000003E-3</v>
+        <v>0.48076923076923078</v>
       </c>
       <c r="AP22" s="1">
         <f t="shared" si="17"/>
@@ -5441,11 +5355,11 @@
       </c>
       <c r="AQ22" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AR22" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="AS22" s="1">
         <f t="shared" si="20"/>
@@ -5461,346 +5375,541 @@
       </c>
       <c r="AV22" s="6">
         <f t="shared" si="23"/>
-        <v>4.807692307692308E-4</v>
-      </c>
-      <c r="AW22" s="6">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="AW22" s="46">
+        <f t="shared" si="24"/>
+        <v>0.72115384615384626</v>
       </c>
     </row>
-    <row r="23" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="7">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>0</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0</v>
-      </c>
-      <c r="K23" s="8">
-        <v>0</v>
-      </c>
-      <c r="L23" s="8">
-        <v>0</v>
-      </c>
-      <c r="M23" s="8">
-        <v>0</v>
-      </c>
-      <c r="N23" s="8">
-        <v>0</v>
-      </c>
-      <c r="O23" s="8">
-        <v>0</v>
-      </c>
-      <c r="P23" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>0</v>
-      </c>
-      <c r="R23" s="8">
-        <v>0</v>
-      </c>
-      <c r="S23" s="8">
-        <v>0</v>
-      </c>
-      <c r="T23" s="8">
-        <v>0</v>
-      </c>
-      <c r="U23" s="8">
-        <v>0</v>
-      </c>
-      <c r="V23" s="8">
-        <v>0</v>
-      </c>
-      <c r="W23" s="9">
-        <v>0</v>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="6">
+        <v>1</v>
       </c>
       <c r="X23" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA23" s="7">
+        <v>16</v>
+      </c>
+      <c r="Z23" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA23" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB23" s="8">
+      <c r="AB23" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC23" s="8">
+      <c r="AC23" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD23" s="8">
+      <c r="AD23" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE23" s="8">
+      <c r="AE23" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AF23" s="8">
+      <c r="AF23" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG23" s="8">
+      <c r="AG23" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH23" s="8">
+      <c r="AH23" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AI23" s="8">
+      <c r="AI23" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AJ23" s="8">
+      <c r="AJ23" s="1">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AK23" s="8">
+      <c r="AK23" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AL23" s="8">
+      <c r="AL23" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AM23" s="8">
+      <c r="AM23" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AN23" s="8">
+      <c r="AN23" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AO23" s="8">
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="AO23" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AP23" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="AP23" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AQ23" s="8">
+      <c r="AQ23" s="1">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AR23" s="8">
+      <c r="AR23" s="1">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AS23" s="8">
+      <c r="AS23" s="1">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="AT23" s="8">
+      <c r="AT23" s="1">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AU23" s="8">
+      <c r="AU23" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AV23" s="9">
+      <c r="AV23" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="AW23" s="6">
-        <v>0</v>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="AW23" s="46">
+        <f t="shared" si="24"/>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="B24" s="7">
-        <f>SUM(B2:B23)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0</v>
+      </c>
+      <c r="N24" s="8">
+        <v>0</v>
+      </c>
+      <c r="O24" s="8">
+        <v>0</v>
+      </c>
+      <c r="P24" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>0</v>
+      </c>
+      <c r="R24" s="8">
+        <v>0</v>
+      </c>
+      <c r="S24" s="8">
+        <v>0</v>
+      </c>
+      <c r="T24" s="8">
+        <v>0</v>
+      </c>
+      <c r="U24" s="8">
+        <v>0</v>
+      </c>
+      <c r="V24" s="8">
+        <v>0</v>
+      </c>
+      <c r="W24" s="9">
+        <v>0</v>
+      </c>
+      <c r="X24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA24" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG24" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AK24" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AM24" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AN24" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AO24" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP24" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AR24" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AS24" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AT24" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AU24" s="1">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AV24" s="6">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AW24" s="47">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <f>SUM(B3:B24)</f>
         <v>7</v>
       </c>
-      <c r="C24" s="8">
-        <f t="shared" ref="C24:W24" si="24">SUM(C2:C23)</f>
+      <c r="C25" s="8">
+        <f t="shared" ref="C25:W25" si="25">SUM(C3:C24)</f>
         <v>80</v>
       </c>
-      <c r="D24" s="8">
-        <f t="shared" si="24"/>
+      <c r="D25" s="8">
+        <f t="shared" si="25"/>
         <v>111</v>
       </c>
-      <c r="E24" s="8">
-        <f t="shared" si="24"/>
+      <c r="E25" s="8">
+        <f t="shared" si="25"/>
         <v>47</v>
       </c>
-      <c r="F24" s="8">
-        <f t="shared" si="24"/>
+      <c r="F25" s="8">
+        <f t="shared" si="25"/>
         <v>261</v>
       </c>
-      <c r="G24" s="8">
-        <f t="shared" si="24"/>
+      <c r="G25" s="8">
+        <f t="shared" si="25"/>
         <v>97</v>
       </c>
-      <c r="H24" s="8">
-        <f t="shared" si="24"/>
+      <c r="H25" s="8">
+        <f t="shared" si="25"/>
         <v>15</v>
       </c>
-      <c r="I24" s="8">
-        <f t="shared" si="24"/>
+      <c r="I25" s="8">
+        <f t="shared" si="25"/>
         <v>63</v>
       </c>
-      <c r="J24" s="8">
-        <f t="shared" si="24"/>
+      <c r="J25" s="8">
+        <f t="shared" si="25"/>
         <v>114</v>
       </c>
-      <c r="K24" s="8">
-        <f t="shared" si="24"/>
+      <c r="K25" s="8">
+        <f t="shared" si="25"/>
         <v>71</v>
       </c>
-      <c r="L24" s="8">
-        <f t="shared" si="24"/>
+      <c r="L25" s="8">
+        <f t="shared" si="25"/>
         <v>48</v>
       </c>
-      <c r="M24" s="8">
-        <f t="shared" si="24"/>
+      <c r="M25" s="8">
+        <f t="shared" si="25"/>
         <v>218</v>
       </c>
-      <c r="N24" s="8">
-        <f t="shared" si="24"/>
+      <c r="N25" s="8">
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
-      <c r="O24" s="8">
-        <f t="shared" si="24"/>
+      <c r="O25" s="8">
+        <f t="shared" si="25"/>
         <v>398</v>
       </c>
-      <c r="P24" s="8">
-        <f t="shared" si="24"/>
+      <c r="P25" s="8">
+        <f t="shared" si="25"/>
         <v>86</v>
       </c>
-      <c r="Q24" s="8">
-        <f t="shared" si="24"/>
+      <c r="Q25" s="8">
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
-      <c r="R24" s="8">
-        <f t="shared" si="24"/>
+      <c r="R25" s="8">
+        <f t="shared" si="25"/>
         <v>362</v>
       </c>
-      <c r="S24" s="8">
-        <f t="shared" si="24"/>
+      <c r="S25" s="8">
+        <f t="shared" si="25"/>
         <v>59</v>
       </c>
-      <c r="T24" s="8">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="U24" s="8">
-        <f t="shared" si="24"/>
+      <c r="T25" s="8">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="8">
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
-      <c r="V24" s="8">
-        <f t="shared" si="24"/>
+      <c r="V25" s="8">
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
-      <c r="W24" s="8">
-        <f t="shared" si="24"/>
+      <c r="W25" s="8">
+        <f t="shared" si="25"/>
         <v>24</v>
       </c>
-      <c r="X24" s="10">
-        <f>SUM(X2:X23)</f>
+      <c r="X25" s="10">
+        <f>SUM(X3:X24)</f>
         <v>2080</v>
       </c>
-      <c r="AA24" s="7">
-        <v>7</v>
-      </c>
-      <c r="AB24" s="8">
-        <v>80</v>
-      </c>
-      <c r="AC24" s="8">
-        <v>111</v>
-      </c>
-      <c r="AD24" s="8">
-        <v>47</v>
-      </c>
-      <c r="AE24" s="8">
-        <v>261</v>
-      </c>
-      <c r="AF24" s="8">
-        <v>97</v>
-      </c>
-      <c r="AG24" s="8">
-        <v>15</v>
-      </c>
-      <c r="AH24" s="8">
-        <v>63</v>
-      </c>
-      <c r="AI24" s="8">
-        <v>114</v>
-      </c>
-      <c r="AJ24" s="8">
-        <v>71</v>
-      </c>
-      <c r="AK24" s="8">
-        <v>48</v>
-      </c>
-      <c r="AL24" s="8">
-        <v>218</v>
-      </c>
-      <c r="AM24" s="8">
-        <v>4</v>
-      </c>
-      <c r="AN24" s="8">
-        <v>398</v>
-      </c>
-      <c r="AO24" s="8">
-        <v>86</v>
-      </c>
-      <c r="AP24" s="8">
-        <v>2</v>
-      </c>
-      <c r="AQ24" s="8">
-        <v>362</v>
-      </c>
-      <c r="AR24" s="8">
-        <v>59</v>
-      </c>
-      <c r="AS24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="8">
-        <v>10</v>
-      </c>
-      <c r="AU24" s="8">
-        <v>3</v>
-      </c>
-      <c r="AV24" s="8">
-        <v>24</v>
-      </c>
-      <c r="AW24" s="10">
-        <v>2080</v>
+      <c r="AA25" s="35">
+        <f>SUM(AA3:AA24)</f>
+        <v>0.33653846153846156</v>
+      </c>
+      <c r="AB25" s="36">
+        <f t="shared" ref="AB25:AV25" si="26">SUM(AB3:AB24)</f>
+        <v>3.8461538461538467</v>
+      </c>
+      <c r="AC25" s="36">
+        <f t="shared" si="26"/>
+        <v>5.3365384615384626</v>
+      </c>
+      <c r="AD25" s="36">
+        <f t="shared" si="26"/>
+        <v>2.2596153846153846</v>
+      </c>
+      <c r="AE25" s="36">
+        <f t="shared" si="26"/>
+        <v>12.548076923076923</v>
+      </c>
+      <c r="AF25" s="36">
+        <f t="shared" si="26"/>
+        <v>4.6634615384615392</v>
+      </c>
+      <c r="AG25" s="36">
+        <f t="shared" si="26"/>
+        <v>0.72115384615384637</v>
+      </c>
+      <c r="AH25" s="36">
+        <f t="shared" si="26"/>
+        <v>3.0288461538461542</v>
+      </c>
+      <c r="AI25" s="36">
+        <f t="shared" si="26"/>
+        <v>5.4807692307692308</v>
+      </c>
+      <c r="AJ25" s="36">
+        <f t="shared" si="26"/>
+        <v>3.4134615384615388</v>
+      </c>
+      <c r="AK25" s="36">
+        <f t="shared" si="26"/>
+        <v>2.3076923076923079</v>
+      </c>
+      <c r="AL25" s="36">
+        <f t="shared" si="26"/>
+        <v>10.480769230769232</v>
+      </c>
+      <c r="AM25" s="36">
+        <f t="shared" si="26"/>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="AN25" s="36">
+        <f t="shared" si="26"/>
+        <v>19.134615384615383</v>
+      </c>
+      <c r="AO25" s="36">
+        <f t="shared" si="26"/>
+        <v>4.134615384615385</v>
+      </c>
+      <c r="AP25" s="36">
+        <f t="shared" si="26"/>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="AQ25" s="36">
+        <f t="shared" si="26"/>
+        <v>17.403846153846157</v>
+      </c>
+      <c r="AR25" s="36">
+        <f t="shared" si="26"/>
+        <v>2.8365384615384612</v>
+      </c>
+      <c r="AS25" s="36">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="AT25" s="36">
+        <f t="shared" si="26"/>
+        <v>0.48076923076923084</v>
+      </c>
+      <c r="AU25" s="36">
+        <f t="shared" si="26"/>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="AV25" s="44">
+        <f t="shared" si="26"/>
+        <v>1.153846153846154</v>
+      </c>
+      <c r="AW25" s="48">
+        <f>SUM(AW3:AW24)</f>
+        <v>99.999999999999986</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AA2:AV23">
+  <conditionalFormatting sqref="AA3:AV24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
he rehecho la matriz de usos especificos para agruparla por usos generales y que se pueda interpretar mejor en la memoria
</commit_message>
<xml_diff>
--- a/Excel/matriz_tabla_contingencia.xlsx
+++ b/Excel/matriz_tabla_contingencia.xlsx
@@ -15,6 +15,9 @@
     <sheet name="USOS_GENERAL" sheetId="1" r:id="rId1"/>
     <sheet name="USOS_ESPECIFICOS" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">USOS_ESPECIFICOS!$AZ$2:$BW$2</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="43">
   <si>
     <t>Agrario</t>
   </si>
@@ -190,12 +193,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD88B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -380,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -462,6 +495,141 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +639,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFD88B"/>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFCC99FF"/>
+      <color rgb="FFFFCC66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1818,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW25"/>
+  <dimension ref="A1:BX25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL28" sqref="AL28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AY3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BY1" sqref="AZ1:BY26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,10 +2010,15 @@
     <col min="19" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="48" width="5" customWidth="1"/>
+    <col min="50" max="50" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="75" width="5" customWidth="1"/>
+    <col min="76" max="76" width="7.28515625" customWidth="1"/>
+    <col min="77" max="77" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:49" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:76" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>26</v>
       </c>
@@ -1981,8 +2157,77 @@
       <c r="AV2" s="39" t="s">
         <v>11</v>
       </c>
+      <c r="BA2" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB2" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC2" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD2" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE2" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF2" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="BG2" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH2" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="BI2" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ2" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="BK2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="BL2" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="BM2" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="BN2" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO2" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="BP2" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="BQ2" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="BR2" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="BS2" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="BU2" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="BV2" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="BW2" s="57" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -2151,8 +2396,103 @@
         <f>SUM(AA3:AV3)</f>
         <v>8.6538461538461533</v>
       </c>
+      <c r="BA3" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB3" s="72">
+        <f>E6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC3" s="73">
+        <f>P6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD3" s="73">
+        <f>T6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE3" s="73">
+        <f>U6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF3" s="73">
+        <f>V6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG3" s="74">
+        <f>W6/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BH3" s="75">
+        <f>F6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI3" s="72">
+        <f>G6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="73">
+        <f>J6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK3" s="73">
+        <f>K6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL3" s="73">
+        <f>L6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM3" s="73">
+        <f>N6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN3" s="73">
+        <f>O6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO3" s="74">
+        <f>S6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP3" s="72">
+        <f>B6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="73">
+        <f>D6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR3" s="73">
+        <f>H6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS3" s="74">
+        <f>I6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT3" s="73">
+        <f>C6/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BU3" s="73">
+        <f>M6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV3" s="73">
+        <f>Q6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW3" s="74">
+        <f>R6/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX3" s="88">
+        <f>SUM(BB3:BW3)</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -2321,8 +2661,103 @@
         <f t="shared" ref="AW4:AW24" si="24">SUM(AA4:AV4)</f>
         <v>0.19230769230769232</v>
       </c>
+      <c r="BA4" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB4" s="76">
+        <f>E17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC4" s="77">
+        <f>P17/$X$25*100</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BD4" s="77">
+        <f>T17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE4" s="77">
+        <f>U17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BF4" s="77">
+        <f>V17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG4" s="78">
+        <f>W17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH4" s="79">
+        <f>F17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BI4" s="76">
+        <f>G17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="77">
+        <f>J17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK4" s="77">
+        <f>K17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL4" s="77">
+        <f>L17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BM4" s="77">
+        <f>N17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN4" s="77">
+        <f>O17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO4" s="78">
+        <f>S17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP4" s="76">
+        <f>B17/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BQ4" s="77">
+        <f>D17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BR4" s="77">
+        <f>H17/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BS4" s="78">
+        <f>I17/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT4" s="77">
+        <f>C17/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BU4" s="77">
+        <f>M17/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BV4" s="77">
+        <f>Q17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BW4" s="78">
+        <f>R17/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX4" s="89">
+        <f>SUM(BB4:BW4)</f>
+        <v>1.2500000000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -2491,8 +2926,103 @@
         <f t="shared" si="24"/>
         <v>11.538461538461538</v>
       </c>
+      <c r="BA5" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB5" s="76">
+        <f>E21/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BC5" s="77">
+        <f>P21/$X$25*100</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="BD5" s="77">
+        <f>T21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE5" s="77">
+        <f>U21/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BF5" s="77">
+        <f>V21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG5" s="78">
+        <f>W21/$X$25*100</f>
+        <v>0.72115384615384615</v>
+      </c>
+      <c r="BH5" s="79">
+        <f>F21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI5" s="76">
+        <f>G21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="77">
+        <f>J21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK5" s="77">
+        <f>K21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL5" s="77">
+        <f>L21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM5" s="77">
+        <f>N21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN5" s="77">
+        <f>O21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO5" s="78">
+        <f>S21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP5" s="76">
+        <f>B21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="77">
+        <f>D21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR5" s="77">
+        <f>H21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS5" s="78">
+        <f>I21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT5" s="77">
+        <f>C21/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BU5" s="77">
+        <f>M21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV5" s="77">
+        <f>Q21/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW5" s="78">
+        <f>R21/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX5" s="89">
+        <f>SUM(BB5:BW5)</f>
+        <v>1.5384615384615385</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2661,8 +3191,103 @@
         <f t="shared" si="24"/>
         <v>9.6153846153846159E-2</v>
       </c>
+      <c r="BA6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB6" s="76">
+        <f>E22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC6" s="77">
+        <f>P22/$X$25*100</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="BD6" s="77">
+        <f>T22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE6" s="77">
+        <f>U22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF6" s="77">
+        <f>V22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG6" s="78">
+        <f>W22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH6" s="79">
+        <f>F22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI6" s="76">
+        <f>G22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="77">
+        <f>J22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK6" s="77">
+        <f>K22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL6" s="77">
+        <f>L22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM6" s="77">
+        <f>N22/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BN6" s="77">
+        <f>O22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO6" s="78">
+        <f>S22/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BP6" s="76">
+        <f>B22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="77">
+        <f>D22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR6" s="77">
+        <f>H22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS6" s="78">
+        <f>I22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT6" s="77">
+        <f>C22/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BU6" s="77">
+        <f>M22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV6" s="77">
+        <f>Q22/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW6" s="78">
+        <f>R22/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX6" s="89">
+        <f>SUM(BB6:BW6)</f>
+        <v>0.72115384615384626</v>
+      </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2831,8 +3456,103 @@
         <f t="shared" si="24"/>
         <v>13.942307692307692</v>
       </c>
+      <c r="BA7" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB7" s="76">
+        <f>E23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC7" s="77">
+        <f>P23/$X$25*100</f>
+        <v>0.625</v>
+      </c>
+      <c r="BD7" s="77">
+        <f>T23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE7" s="77">
+        <f>U23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF7" s="77">
+        <f>V23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG7" s="78">
+        <f>W23/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BH7" s="79">
+        <f>F23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI7" s="76">
+        <f>G23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="77">
+        <f>J23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK7" s="77">
+        <f>K23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL7" s="77">
+        <f>L23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM7" s="77">
+        <f>N23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN7" s="77">
+        <f>O23/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BO7" s="78">
+        <f>S23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP7" s="76">
+        <f>B23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="77">
+        <f>D23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR7" s="77">
+        <f>H23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS7" s="78">
+        <f>I23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT7" s="77">
+        <f>C23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU7" s="77">
+        <f>M23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV7" s="77">
+        <f>Q23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW7" s="78">
+        <f>R23/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX7" s="89">
+        <f>SUM(BB7:BW7)</f>
+        <v>0.76923076923076927</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3001,8 +3721,103 @@
         <f t="shared" si="24"/>
         <v>2.6923076923076925</v>
       </c>
+      <c r="BA8" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB8" s="80">
+        <f>E24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC8" s="81">
+        <f>P24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD8" s="81">
+        <f>T24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE8" s="81">
+        <f>U24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF8" s="81">
+        <f>V24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG8" s="82">
+        <f>W24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH8" s="83">
+        <f>F24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI8" s="80">
+        <f>G24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="81">
+        <f>J24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK8" s="81">
+        <f>K24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL8" s="81">
+        <f>L24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM8" s="81">
+        <f>N24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN8" s="81">
+        <f>O24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO8" s="82">
+        <f>S24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP8" s="80">
+        <f>B24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="81">
+        <f>D24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR8" s="81">
+        <f>H24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS8" s="82">
+        <f>I24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT8" s="81">
+        <f>C24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU8" s="81">
+        <f>M24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV8" s="81">
+        <f>Q24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW8" s="82">
+        <f>R24/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX8" s="90">
+        <f>SUM(BB8:BW8)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -3171,8 +3986,103 @@
         <f t="shared" si="24"/>
         <v>0.43269230769230771</v>
       </c>
+      <c r="BA9" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB9" s="84">
+        <f>E7/$X$25*100</f>
+        <v>0.52884615384615385</v>
+      </c>
+      <c r="BC9" s="85">
+        <f>P7/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BD9" s="85">
+        <f>T7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE9" s="85">
+        <f>U7/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BF9" s="85">
+        <f>V7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG9" s="86">
+        <f>W7/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BH9" s="87">
+        <f>F7/$X$25*100</f>
+        <v>11.057692307692307</v>
+      </c>
+      <c r="BI9" s="84">
+        <f>G7/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BJ9" s="85">
+        <f>J7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK9" s="85">
+        <f>K7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL9" s="85">
+        <f>L7/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BM9" s="85">
+        <f>N7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN9" s="85">
+        <f>O7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO9" s="86">
+        <f>S7/$X$25*100</f>
+        <v>0.24038461538461539</v>
+      </c>
+      <c r="BP9" s="84">
+        <f>B7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="85">
+        <f>D7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR9" s="85">
+        <f>H7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS9" s="86">
+        <f>I7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT9" s="85">
+        <f>C7/$X$25*100</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BU9" s="85">
+        <f>M7/$X$25*100</f>
+        <v>0.57692307692307698</v>
+      </c>
+      <c r="BV9" s="85">
+        <f>Q7/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW9" s="86">
+        <f>R7/$X$25*100</f>
+        <v>0.625</v>
+      </c>
+      <c r="BX9" s="91">
+        <f>SUM(BB9:BW9)</f>
+        <v>13.942307692307692</v>
+      </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -3341,8 +4251,103 @@
         <f t="shared" si="24"/>
         <v>0.24038461538461539</v>
       </c>
+      <c r="BA10" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB10" s="72">
+        <f>E8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC10" s="73">
+        <f>P8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD10" s="73">
+        <f>T8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE10" s="73">
+        <f>U8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF10" s="73">
+        <f>V8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG10" s="74">
+        <f>W8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH10" s="75">
+        <f>F8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI10" s="72">
+        <f>G8/$X$25*100</f>
+        <v>2.4519230769230771</v>
+      </c>
+      <c r="BJ10" s="73">
+        <f>J8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK10" s="73">
+        <f>K8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL10" s="73">
+        <f>L8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM10" s="73">
+        <f>N8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN10" s="73">
+        <f>O8/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BO10" s="74">
+        <f>S8/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BP10" s="72">
+        <f>B8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="73">
+        <f>D8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR10" s="73">
+        <f>H8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS10" s="74">
+        <f>I8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT10" s="73">
+        <f>C8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU10" s="73">
+        <f>M8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV10" s="73">
+        <f>Q8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW10" s="74">
+        <f>R8/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX10" s="88">
+        <f>SUM(BB10:BW10)</f>
+        <v>2.6923076923076925</v>
+      </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -3511,8 +4516,103 @@
         <f t="shared" si="24"/>
         <v>5.6730769230769234</v>
       </c>
+      <c r="BA11" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB11" s="76">
+        <f>E11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC11" s="77">
+        <f>P11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD11" s="77">
+        <f>T11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE11" s="77">
+        <f>U11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF11" s="77">
+        <f>V11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG11" s="78">
+        <f>W11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH11" s="79">
+        <f>F11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI11" s="76">
+        <f>G11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="77">
+        <f>J11/$X$25*100</f>
+        <v>5.384615384615385</v>
+      </c>
+      <c r="BK11" s="77">
+        <f>K11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL11" s="77">
+        <f>L11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM11" s="77">
+        <f>N11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN11" s="77">
+        <f>O11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO11" s="78">
+        <f>S11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP11" s="76">
+        <f>B11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ11" s="77">
+        <f>D11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR11" s="77">
+        <f>H11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS11" s="78">
+        <f>I11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT11" s="77">
+        <f>C11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU11" s="77">
+        <f>M11/$X$25*100</f>
+        <v>0.28846153846153849</v>
+      </c>
+      <c r="BV11" s="77">
+        <f>Q11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW11" s="78">
+        <f>R11/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX11" s="89">
+        <f>SUM(BB11:BW11)</f>
+        <v>5.6730769230769234</v>
+      </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -3681,8 +4781,103 @@
         <f t="shared" si="24"/>
         <v>2.2115384615384617</v>
       </c>
+      <c r="BA12" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB12" s="76">
+        <f>E12/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BC12" s="77">
+        <f>P12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD12" s="77">
+        <f>T12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE12" s="77">
+        <f>U12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF12" s="77">
+        <f>V12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG12" s="78">
+        <f>W12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH12" s="79">
+        <f>F12/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BI12" s="76">
+        <f>G12/$X$25*100</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="BJ12" s="77">
+        <f>J12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK12" s="77">
+        <f>K12/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BL12" s="77">
+        <f>L12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM12" s="77">
+        <f>N12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN12" s="77">
+        <f>O12/$X$25*100</f>
+        <v>0.96153846153846156</v>
+      </c>
+      <c r="BO12" s="78">
+        <f>S12/$X$25*100</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BP12" s="76">
+        <f>B12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="77">
+        <f>D12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR12" s="77">
+        <f>H12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS12" s="78">
+        <f>I12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT12" s="77">
+        <f>C12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU12" s="77">
+        <f>M12/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BV12" s="77">
+        <f>Q12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW12" s="78">
+        <f>R12/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX12" s="89">
+        <f>SUM(BB12:BW12)</f>
+        <v>2.2115384615384617</v>
+      </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -3851,8 +5046,103 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
+      <c r="BA13" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB13" s="76">
+        <f>E13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC13" s="77">
+        <f>P13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD13" s="77">
+        <f>T13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE13" s="77">
+        <f>U13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF13" s="77">
+        <f>V13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG13" s="78">
+        <f>W13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH13" s="79">
+        <f>F13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI13" s="76">
+        <f>G13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ13" s="77">
+        <f>J13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK13" s="77">
+        <f>K13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL13" s="77">
+        <f>L13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM13" s="77">
+        <f>N13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN13" s="77">
+        <f>O13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO13" s="78">
+        <f>S13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP13" s="76">
+        <f>B13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ13" s="77">
+        <f>D13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR13" s="77">
+        <f>H13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS13" s="78">
+        <f>I13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT13" s="77">
+        <f>C13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU13" s="77">
+        <f>M13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV13" s="77">
+        <f>Q13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW13" s="78">
+        <f>R13/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX13" s="92">
+        <f>SUM(BB13:BW13)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -4021,8 +5311,103 @@
         <f t="shared" si="24"/>
         <v>2.5480769230769229</v>
       </c>
+      <c r="BA14" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB14" s="76">
+        <f>E15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC14" s="77">
+        <f>P15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD14" s="77">
+        <f>T15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE14" s="77">
+        <f>U15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF14" s="77">
+        <f>V15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG14" s="78">
+        <f>W15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH14" s="79">
+        <f>F15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI14" s="76">
+        <f>G15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ14" s="77">
+        <f>J15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK14" s="77">
+        <f>K15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL14" s="77">
+        <f>L15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM14" s="77">
+        <f>N15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN14" s="77">
+        <f>O15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO14" s="78">
+        <f>S15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP14" s="76">
+        <f>B15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="77">
+        <f>D15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR14" s="77">
+        <f>H15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS14" s="78">
+        <f>I15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT14" s="77">
+        <f>C15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU14" s="77">
+        <f>M15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV14" s="77">
+        <f>Q15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW14" s="78">
+        <f>R15/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX14" s="89">
+        <f>SUM(BB14:BW14)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4191,8 +5576,103 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
+      <c r="BA15" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB15" s="76">
+        <f>E16/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BC15" s="77">
+        <f>P16/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BD15" s="77">
+        <f>T16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE15" s="77">
+        <f>U16/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BF15" s="77">
+        <f>V16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG15" s="78">
+        <f>W16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH15" s="79">
+        <f>F16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI15" s="76">
+        <f>G16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ15" s="77">
+        <f>J16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK15" s="77">
+        <f>K16/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BL15" s="77">
+        <f>L16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM15" s="77">
+        <f>N16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN15" s="77">
+        <f>O16/$X$25*100</f>
+        <v>11.875</v>
+      </c>
+      <c r="BO15" s="78">
+        <f>S16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP15" s="76">
+        <f>B16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ15" s="77">
+        <f>D16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR15" s="77">
+        <f>H16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS15" s="78">
+        <f>I16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT15" s="77">
+        <f>C16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU15" s="77">
+        <f>M16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV15" s="77">
+        <f>Q16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW15" s="78">
+        <f>R16/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX15" s="92">
+        <f>SUM(BB15:BW15)</f>
+        <v>12.211538461538462</v>
+      </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
@@ -4361,8 +5841,103 @@
         <f t="shared" si="24"/>
         <v>12.211538461538463</v>
       </c>
+      <c r="BA16" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB16" s="80">
+        <f>E20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC16" s="81">
+        <f>P20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD16" s="81">
+        <f>T20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE16" s="81">
+        <f>U20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF16" s="81">
+        <f>V20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG16" s="82">
+        <f>W20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH16" s="83">
+        <f>F20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI16" s="80">
+        <f>G20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="81">
+        <f>J20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK16" s="81">
+        <f>K20/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BL16" s="81">
+        <f>L20/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BM16" s="81">
+        <f>N20/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BN16" s="81">
+        <f>O20/$X$25*100</f>
+        <v>0.33653846153846156</v>
+      </c>
+      <c r="BO16" s="82">
+        <f>S20/$X$25*100</f>
+        <v>0.28846153846153849</v>
+      </c>
+      <c r="BP16" s="80">
+        <f>B20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ16" s="81">
+        <f>D20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR16" s="81">
+        <f>H20/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BS16" s="82">
+        <f>I20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT16" s="81">
+        <f>C20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU16" s="81">
+        <f>M20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV16" s="81">
+        <f>Q20/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW16" s="82">
+        <f>R20/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX16" s="90">
+        <f>SUM(BB16:BW16)</f>
+        <v>1.153846153846154</v>
+      </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -4531,8 +6106,103 @@
         <f t="shared" si="24"/>
         <v>1.2500000000000002</v>
       </c>
+      <c r="BA17" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB17" s="76">
+        <f>E3/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BC17" s="77">
+        <f>P3/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BD17" s="77">
+        <f>T3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE17" s="77">
+        <f>U3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF17" s="77">
+        <f>V3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG17" s="78">
+        <f>W3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH17" s="79">
+        <f>F3/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BI17" s="76">
+        <f>G3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ17" s="77">
+        <f>J3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK17" s="77">
+        <f>K3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL17" s="77">
+        <f>L3/$X$25*100</f>
+        <v>1.1057692307692308</v>
+      </c>
+      <c r="BM17" s="77">
+        <f>N3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN17" s="77">
+        <f>O3/$X$25*100</f>
+        <v>0.28846153846153849</v>
+      </c>
+      <c r="BO17" s="78">
+        <f>S3/$X$25*100</f>
+        <v>0.625</v>
+      </c>
+      <c r="BP17" s="76">
+        <f>B3/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BQ17" s="77">
+        <f>D3/$X$25*100</f>
+        <v>2.0192307692307692</v>
+      </c>
+      <c r="BR17" s="77">
+        <f>H3/$X$25*100</f>
+        <v>0.33653846153846156</v>
+      </c>
+      <c r="BS17" s="78">
+        <f>I3/$X$25*100</f>
+        <v>1.7307692307692308</v>
+      </c>
+      <c r="BT17" s="77">
+        <f>C3/$X$25*100</f>
+        <v>0.24038461538461539</v>
+      </c>
+      <c r="BU17" s="77">
+        <f>M3/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BV17" s="77">
+        <f>Q3/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW17" s="78">
+        <f>R3/$X$25*100</f>
+        <v>1.7307692307692308</v>
+      </c>
+      <c r="BX17" s="89">
+        <f>SUM(BB17:BW17)</f>
+        <v>8.6538461538461533</v>
+      </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -4701,8 +6371,103 @@
         <f t="shared" si="24"/>
         <v>9.6153846153846159E-2</v>
       </c>
+      <c r="BA18" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB18" s="76">
+        <f>E5/$X$25*100</f>
+        <v>0.43269230769230771</v>
+      </c>
+      <c r="BC18" s="77">
+        <f>P5/$X$25*100</f>
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="BD18" s="77">
+        <f>T5/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE18" s="77">
+        <f>U5/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BF18" s="77">
+        <f>V5/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BG18" s="78">
+        <f>W5/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BH18" s="79">
+        <f>F5/$X$25*100</f>
+        <v>0.72115384615384615</v>
+      </c>
+      <c r="BI18" s="76">
+        <f>G5/$X$25*100</f>
+        <v>1.3461538461538463</v>
+      </c>
+      <c r="BJ18" s="77">
+        <f>J5/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK18" s="77">
+        <f>K5/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BL18" s="77">
+        <f>L5/$X$25*100</f>
+        <v>0.43269230769230771</v>
+      </c>
+      <c r="BM18" s="77">
+        <f>N5/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN18" s="77">
+        <f>O5/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO18" s="78">
+        <f>S5/$X$25*100</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="BP18" s="76">
+        <f>B5/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BQ18" s="77">
+        <f>D5/$X$25*100</f>
+        <v>2.7403846153846154</v>
+      </c>
+      <c r="BR18" s="77">
+        <f>H5/$X$25*100</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BS18" s="78">
+        <f>I5/$X$25*100</f>
+        <v>0.52884615384615385</v>
+      </c>
+      <c r="BT18" s="77">
+        <f>C5/$X$25*100</f>
+        <v>0.86538461538461542</v>
+      </c>
+      <c r="BU18" s="77">
+        <f>M5/$X$25*100</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BV18" s="77">
+        <f>Q5/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW18" s="78">
+        <f>R5/$X$25*100</f>
+        <v>2.2115384615384617</v>
+      </c>
+      <c r="BX18" s="89">
+        <f>SUM(BB18:BW18)</f>
+        <v>11.538461538461538</v>
+      </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
@@ -4871,8 +6636,103 @@
         <f t="shared" si="24"/>
         <v>34.038461538461533</v>
       </c>
+      <c r="BA19" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB19" s="76">
+        <f>E9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC19" s="77">
+        <f>P9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD19" s="77">
+        <f>T9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE19" s="77">
+        <f>U9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF19" s="77">
+        <f>V9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG19" s="78">
+        <f>W9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH19" s="79">
+        <f>F9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI19" s="76">
+        <f>G9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="77">
+        <f>J9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK19" s="77">
+        <f>K9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL19" s="77">
+        <f>L9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM19" s="77">
+        <f>N9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN19" s="77">
+        <f>O9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO19" s="78">
+        <f>S9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP19" s="76">
+        <f>B9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ19" s="77">
+        <f>D9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR19" s="77">
+        <f>H9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS19" s="78">
+        <f>I9/$X$25*100</f>
+        <v>0.43269230769230771</v>
+      </c>
+      <c r="BT19" s="77">
+        <f>C9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU19" s="77">
+        <f>M9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV19" s="77">
+        <f>Q9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW19" s="78">
+        <f>R9/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX19" s="89">
+        <f>SUM(BB19:BW19)</f>
+        <v>0.43269230769230771</v>
+      </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
@@ -5041,8 +6901,103 @@
         <f t="shared" si="24"/>
         <v>1.153846153846154</v>
       </c>
+      <c r="BA20" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB20" s="76">
+        <f>E10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC20" s="77">
+        <f>P10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD20" s="77">
+        <f>T10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE20" s="77">
+        <f>U10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF20" s="77">
+        <f>V10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG20" s="78">
+        <f>W10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH20" s="79">
+        <f>F10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI20" s="76">
+        <f>G10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ20" s="77">
+        <f>J10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK20" s="77">
+        <f>K10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL20" s="77">
+        <f>L10/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BM20" s="77">
+        <f>N10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN20" s="77">
+        <f>O10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO20" s="78">
+        <f>S10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP20" s="76">
+        <f>B10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ20" s="77">
+        <f>D10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR20" s="77">
+        <f>H10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS20" s="78">
+        <f>I10/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BT20" s="77">
+        <f>C10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BU20" s="77">
+        <f>M10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV20" s="77">
+        <f>Q10/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW20" s="78">
+        <f>R10/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX20" s="89">
+        <f>SUM(BB20:BW20)</f>
+        <v>0.24038461538461539</v>
+      </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -5211,8 +7166,103 @@
         <f t="shared" si="24"/>
         <v>1.5384615384615385</v>
       </c>
+      <c r="BA21" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB21" s="72">
+        <f>E4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC21" s="73">
+        <f>P4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD21" s="73">
+        <f>T4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE21" s="73">
+        <f>U4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF21" s="73">
+        <f>V4/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BG21" s="74">
+        <f>W4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH21" s="75">
+        <f>F4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI21" s="72">
+        <f>G4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ21" s="73">
+        <f>J4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK21" s="73">
+        <f>K4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL21" s="73">
+        <f>L4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM21" s="73">
+        <f>N4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN21" s="73">
+        <f>O4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO21" s="74">
+        <f>S4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP21" s="72">
+        <f>B4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ21" s="73">
+        <f>D4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR21" s="73">
+        <f>H4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS21" s="74">
+        <f>I4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT21" s="73">
+        <f>C4/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BU21" s="73">
+        <f>M4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV21" s="73">
+        <f>Q4/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW21" s="74">
+        <f>R4/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX21" s="88">
+        <f>SUM(BB21:BW21)</f>
+        <v>0.19230769230769232</v>
+      </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -5381,8 +7431,103 @@
         <f t="shared" si="24"/>
         <v>0.72115384615384626</v>
       </c>
+      <c r="BA22" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB22" s="76">
+        <f>E14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC22" s="77">
+        <f>P14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD22" s="77">
+        <f>T14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE22" s="77">
+        <f>U14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF22" s="77">
+        <f>V14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG22" s="78">
+        <f>W14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH22" s="79">
+        <f>F14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI22" s="76">
+        <f>G14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ22" s="77">
+        <f>J14/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BK22" s="77">
+        <f>K14/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BL22" s="77">
+        <f>L14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM22" s="77">
+        <f>N14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN22" s="77">
+        <f>O14/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BO22" s="78">
+        <f>S14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP22" s="76">
+        <f>B14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ22" s="77">
+        <f>D14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR22" s="77">
+        <f>H14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS22" s="78">
+        <f>I14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT22" s="77">
+        <f>C14/$X$25*100</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BU22" s="77">
+        <f>M14/$X$25*100</f>
+        <v>2.1634615384615383</v>
+      </c>
+      <c r="BV22" s="77">
+        <f>Q14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW22" s="78">
+        <f>R14/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BX22" s="89">
+        <f>SUM(BB22:BW22)</f>
+        <v>2.5480769230769229</v>
+      </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -5551,8 +7696,103 @@
         <f t="shared" si="24"/>
         <v>0.76923076923076927</v>
       </c>
+      <c r="BA23" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB23" s="76">
+        <f>E18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BC23" s="77">
+        <f>P18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BD23" s="77">
+        <f>T18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE23" s="77">
+        <f>U18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF23" s="77">
+        <f>V18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BG23" s="78">
+        <f>W18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BH23" s="79">
+        <f>F18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BI23" s="76">
+        <f>G18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BJ23" s="77">
+        <f>J18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK23" s="77">
+        <f>K18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BL23" s="77">
+        <f>L18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BM23" s="77">
+        <f>N18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN23" s="77">
+        <f>O18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BO23" s="78">
+        <f>S18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BP23" s="76">
+        <f>B18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ23" s="77">
+        <f>D18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BR23" s="77">
+        <f>H18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BS23" s="78">
+        <f>I18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BT23" s="77">
+        <f>C18/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BU23" s="77">
+        <f>M18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BV23" s="77">
+        <f>Q18/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BW23" s="78">
+        <f>R18/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BX23" s="89">
+        <f>SUM(BB23:BW23)</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
@@ -5721,8 +7961,103 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
+      <c r="BA24" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB24" s="80">
+        <f>E19/$X$25*100</f>
+        <v>0.91346153846153855</v>
+      </c>
+      <c r="BC24" s="81">
+        <f>P19/$X$25*100</f>
+        <v>1.2019230769230771</v>
+      </c>
+      <c r="BD24" s="81">
+        <f>T19/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BE24" s="81">
+        <f>U19/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BF24" s="81">
+        <f>V19/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BG24" s="82">
+        <f>W19/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BH24" s="83">
+        <f>F19/$X$25*100</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BI24" s="80">
+        <f>G19/$X$25*100</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BJ24" s="81">
+        <f>J19/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BK24" s="81">
+        <f>K19/$X$25*100</f>
+        <v>2.8846153846153846</v>
+      </c>
+      <c r="BL24" s="81">
+        <f>L19/$X$25*100</f>
+        <v>0.43269230769230771</v>
+      </c>
+      <c r="BM24" s="81">
+        <f>N19/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BN24" s="81">
+        <f>O19/$X$25*100</f>
+        <v>5.2884615384615383</v>
+      </c>
+      <c r="BO24" s="82">
+        <f>S19/$X$25*100</f>
+        <v>0.72115384615384615</v>
+      </c>
+      <c r="BP24" s="80">
+        <f>B19/$X$25*100</f>
+        <v>0</v>
+      </c>
+      <c r="BQ24" s="81">
+        <f>D19/$X$25*100</f>
+        <v>0.52884615384615385</v>
+      </c>
+      <c r="BR24" s="81">
+        <f>H19/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BS24" s="82">
+        <f>I19/$X$25*100</f>
+        <v>0.24038461538461539</v>
+      </c>
+      <c r="BT24" s="81">
+        <f>C19/$X$25*100</f>
+        <v>1.6826923076923077</v>
+      </c>
+      <c r="BU24" s="81">
+        <f>M19/$X$25*100</f>
+        <v>6.8750000000000009</v>
+      </c>
+      <c r="BV24" s="81">
+        <f>Q19/$X$25*100</f>
+        <v>4.807692307692308E-2</v>
+      </c>
+      <c r="BW24" s="82">
+        <f>R19/$X$25*100</f>
+        <v>12.5</v>
+      </c>
+      <c r="BX24" s="93">
+        <f>SUM(BB24:BW24)</f>
+        <v>34.03846153846154</v>
+      </c>
     </row>
-    <row r="25" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
         <f>SUM(B3:B24)</f>
         <v>7</v>
@@ -5907,9 +8242,111 @@
         <f>SUM(AW3:AW24)</f>
         <v>99.999999999999986</v>
       </c>
+      <c r="BB25" s="84">
+        <f>SUM(BB3:BB24)</f>
+        <v>2.259615384615385</v>
+      </c>
+      <c r="BC25" s="85">
+        <f>SUM(BC3:BC24)</f>
+        <v>4.134615384615385</v>
+      </c>
+      <c r="BD25" s="85">
+        <f>SUM(BD3:BD24)</f>
+        <v>0</v>
+      </c>
+      <c r="BE25" s="85">
+        <f>SUM(BE3:BE24)</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="BF25" s="85">
+        <f>SUM(BF3:BF24)</f>
+        <v>0.14423076923076925</v>
+      </c>
+      <c r="BG25" s="86">
+        <f>SUM(BG3:BG24)</f>
+        <v>1.153846153846154</v>
+      </c>
+      <c r="BH25" s="87">
+        <f>SUM(BH3:BH24)</f>
+        <v>12.548076923076923</v>
+      </c>
+      <c r="BI25" s="84">
+        <f>SUM(BI3:BI24)</f>
+        <v>4.6634615384615392</v>
+      </c>
+      <c r="BJ25" s="85">
+        <f>SUM(BJ3:BJ24)</f>
+        <v>5.4807692307692308</v>
+      </c>
+      <c r="BK25" s="85">
+        <f>SUM(BK3:BK24)</f>
+        <v>3.4134615384615383</v>
+      </c>
+      <c r="BL25" s="85">
+        <f>SUM(BL3:BL24)</f>
+        <v>2.3076923076923079</v>
+      </c>
+      <c r="BM25" s="85">
+        <f>SUM(BM3:BM24)</f>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="BN25" s="85">
+        <f>SUM(BN3:BN24)</f>
+        <v>19.134615384615387</v>
+      </c>
+      <c r="BO25" s="86">
+        <f>SUM(BO3:BO24)</f>
+        <v>2.8365384615384617</v>
+      </c>
+      <c r="BP25" s="84">
+        <f>SUM(BP3:BP24)</f>
+        <v>0.33653846153846156</v>
+      </c>
+      <c r="BQ25" s="85">
+        <f>SUM(BQ3:BQ24)</f>
+        <v>5.3365384615384617</v>
+      </c>
+      <c r="BR25" s="85">
+        <f>SUM(BR3:BR24)</f>
+        <v>0.72115384615384626</v>
+      </c>
+      <c r="BS25" s="86">
+        <f>SUM(BS3:BS24)</f>
+        <v>3.0288461538461542</v>
+      </c>
+      <c r="BT25" s="85">
+        <f>SUM(BT3:BT24)</f>
+        <v>3.8461538461538458</v>
+      </c>
+      <c r="BU25" s="85">
+        <f>SUM(BU3:BU24)</f>
+        <v>10.480769230769232</v>
+      </c>
+      <c r="BV25" s="85">
+        <f>SUM(BV3:BV24)</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="BW25" s="86">
+        <f>SUM(BW3:BW24)</f>
+        <v>17.403846153846153</v>
+      </c>
+      <c r="BX25" s="48">
+        <f>SUM(BX3:BX24)</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AA3:AV24">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB3:BW24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>